<commit_message>
Latest Excel version of status doc
</commit_message>
<xml_diff>
--- a/notes/status.xlsx
+++ b/notes/status.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
   <si>
     <t>Y</t>
   </si>
@@ -36,10 +36,13 @@
     <t>&gt;0</t>
   </si>
   <si>
-    <t>N</t>
+    <t>khan2012.py</t>
   </si>
   <si>
-    <t>macqueen1967.py</t>
+    <t>Single column? </t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -68,7 +71,7 @@
       <strike val="0"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,12 +81,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -121,7 +118,7 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
@@ -140,9 +137,6 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -152,11 +146,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IV29"/>
+  <dimension ref="A1:IV65536"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:IV13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:IV8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -166,7 +160,7 @@
     <col min="3" max="3" style="1" width="15.141947115384617" customWidth="1"/>
     <col min="4" max="4" style="1" width="8.999459134615385" customWidth="1"/>
     <col min="5" max="5" style="1" width="9.142307692307693"/>
-    <col min="6" max="6" style="1" width="16.998978365384616" customWidth="1"/>
+    <col min="6" max="6" style="1" width="15.141947115384617" customWidth="1"/>
     <col min="7" max="7" style="1" width="9.142307692307693"/>
     <col min="8" max="8" style="1" width="11.1421875" customWidth="1"/>
     <col min="9" max="256" style="1" width="9.142307692307693"/>
@@ -1869,284 +1863,564 @@
       <c r="IV6" s="3"/>
     </row>
     <row r="7" spans="1:256" ht="13.5">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>ikmeans.py</t>
         </is>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
+      <c r="B7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>~Y</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>TBC</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+      <c r="AU7" s="3"/>
+      <c r="AV7" s="3"/>
+      <c r="AW7" s="3"/>
+      <c r="AX7" s="3"/>
+      <c r="AY7" s="3"/>
+      <c r="AZ7" s="3"/>
+      <c r="BA7" s="3"/>
+      <c r="BB7" s="3"/>
+      <c r="BC7" s="3"/>
+      <c r="BD7" s="3"/>
+      <c r="BE7" s="3"/>
+      <c r="BF7" s="3"/>
+      <c r="BG7" s="3"/>
+      <c r="BH7" s="3"/>
+      <c r="BI7" s="3"/>
+      <c r="BJ7" s="3"/>
+      <c r="BK7" s="3"/>
+      <c r="BL7" s="3"/>
+      <c r="BM7" s="3"/>
+      <c r="BN7" s="3"/>
+      <c r="BO7" s="3"/>
+      <c r="BP7" s="3"/>
+      <c r="BQ7" s="3"/>
+      <c r="BR7" s="3"/>
+      <c r="BS7" s="3"/>
+      <c r="BT7" s="3"/>
+      <c r="BU7" s="3"/>
+      <c r="BV7" s="3"/>
+      <c r="BW7" s="3"/>
+      <c r="BX7" s="3"/>
+      <c r="BY7" s="3"/>
+      <c r="BZ7" s="3"/>
+      <c r="CA7" s="3"/>
+      <c r="CB7" s="3"/>
+      <c r="CC7" s="3"/>
+      <c r="CD7" s="3"/>
+      <c r="CE7" s="3"/>
+      <c r="CF7" s="3"/>
+      <c r="CG7" s="3"/>
+      <c r="CH7" s="3"/>
+      <c r="CI7" s="3"/>
+      <c r="CJ7" s="3"/>
+      <c r="CK7" s="3"/>
+      <c r="CL7" s="3"/>
+      <c r="CM7" s="3"/>
+      <c r="CN7" s="3"/>
+      <c r="CO7" s="3"/>
+      <c r="CP7" s="3"/>
+      <c r="CQ7" s="3"/>
+      <c r="CR7" s="3"/>
+      <c r="CS7" s="3"/>
+      <c r="CT7" s="3"/>
+      <c r="CU7" s="3"/>
+      <c r="CV7" s="3"/>
+      <c r="CW7" s="3"/>
+      <c r="CX7" s="3"/>
+      <c r="CY7" s="3"/>
+      <c r="CZ7" s="3"/>
+      <c r="DA7" s="3"/>
+      <c r="DB7" s="3"/>
+      <c r="DC7" s="3"/>
+      <c r="DD7" s="3"/>
+      <c r="DE7" s="3"/>
+      <c r="DF7" s="3"/>
+      <c r="DG7" s="3"/>
+      <c r="DH7" s="3"/>
+      <c r="DI7" s="3"/>
+      <c r="DJ7" s="3"/>
+      <c r="DK7" s="3"/>
+      <c r="DL7" s="3"/>
+      <c r="DM7" s="3"/>
+      <c r="DN7" s="3"/>
+      <c r="DO7" s="3"/>
+      <c r="DP7" s="3"/>
+      <c r="DQ7" s="3"/>
+      <c r="DR7" s="3"/>
+      <c r="DS7" s="3"/>
+      <c r="DT7" s="3"/>
+      <c r="DU7" s="3"/>
+      <c r="DV7" s="3"/>
+      <c r="DW7" s="3"/>
+      <c r="DX7" s="3"/>
+      <c r="DY7" s="3"/>
+      <c r="DZ7" s="3"/>
+      <c r="EA7" s="3"/>
+      <c r="EB7" s="3"/>
+      <c r="EC7" s="3"/>
+      <c r="ED7" s="3"/>
+      <c r="EE7" s="3"/>
+      <c r="EF7" s="3"/>
+      <c r="EG7" s="3"/>
+      <c r="EH7" s="3"/>
+      <c r="EI7" s="3"/>
+      <c r="EJ7" s="3"/>
+      <c r="EK7" s="3"/>
+      <c r="EL7" s="3"/>
+      <c r="EM7" s="3"/>
+      <c r="EN7" s="3"/>
+      <c r="EO7" s="3"/>
+      <c r="EP7" s="3"/>
+      <c r="EQ7" s="3"/>
+      <c r="ER7" s="3"/>
+      <c r="ES7" s="3"/>
+      <c r="ET7" s="3"/>
+      <c r="EU7" s="3"/>
+      <c r="EV7" s="3"/>
+      <c r="EW7" s="3"/>
+      <c r="EX7" s="3"/>
+      <c r="EY7" s="3"/>
+      <c r="EZ7" s="3"/>
+      <c r="FA7" s="3"/>
+      <c r="FB7" s="3"/>
+      <c r="FC7" s="3"/>
+      <c r="FD7" s="3"/>
+      <c r="FE7" s="3"/>
+      <c r="FF7" s="3"/>
+      <c r="FG7" s="3"/>
+      <c r="FH7" s="3"/>
+      <c r="FI7" s="3"/>
+      <c r="FJ7" s="3"/>
+      <c r="FK7" s="3"/>
+      <c r="FL7" s="3"/>
+      <c r="FM7" s="3"/>
+      <c r="FN7" s="3"/>
+      <c r="FO7" s="3"/>
+      <c r="FP7" s="3"/>
+      <c r="FQ7" s="3"/>
+      <c r="FR7" s="3"/>
+      <c r="FS7" s="3"/>
+      <c r="FT7" s="3"/>
+      <c r="FU7" s="3"/>
+      <c r="FV7" s="3"/>
+      <c r="FW7" s="3"/>
+      <c r="FX7" s="3"/>
+      <c r="FY7" s="3"/>
+      <c r="FZ7" s="3"/>
+      <c r="GA7" s="3"/>
+      <c r="GB7" s="3"/>
+      <c r="GC7" s="3"/>
+      <c r="GD7" s="3"/>
+      <c r="GE7" s="3"/>
+      <c r="GF7" s="3"/>
+      <c r="GG7" s="3"/>
+      <c r="GH7" s="3"/>
+      <c r="GI7" s="3"/>
+      <c r="GJ7" s="3"/>
+      <c r="GK7" s="3"/>
+      <c r="GL7" s="3"/>
+      <c r="GM7" s="3"/>
+      <c r="GN7" s="3"/>
+      <c r="GO7" s="3"/>
+      <c r="GP7" s="3"/>
+      <c r="GQ7" s="3"/>
+      <c r="GR7" s="3"/>
+      <c r="GS7" s="3"/>
+      <c r="GT7" s="3"/>
+      <c r="GU7" s="3"/>
+      <c r="GV7" s="3"/>
+      <c r="GW7" s="3"/>
+      <c r="GX7" s="3"/>
+      <c r="GY7" s="3"/>
+      <c r="GZ7" s="3"/>
+      <c r="HA7" s="3"/>
+      <c r="HB7" s="3"/>
+      <c r="HC7" s="3"/>
+      <c r="HD7" s="3"/>
+      <c r="HE7" s="3"/>
+      <c r="HF7" s="3"/>
+      <c r="HG7" s="3"/>
+      <c r="HH7" s="3"/>
+      <c r="HI7" s="3"/>
+      <c r="HJ7" s="3"/>
+      <c r="HK7" s="3"/>
+      <c r="HL7" s="3"/>
+      <c r="HM7" s="3"/>
+      <c r="HN7" s="3"/>
+      <c r="HO7" s="3"/>
+      <c r="HP7" s="3"/>
+      <c r="HQ7" s="3"/>
+      <c r="HR7" s="3"/>
+      <c r="HS7" s="3"/>
+      <c r="HT7" s="3"/>
+      <c r="HU7" s="3"/>
+      <c r="HV7" s="3"/>
+      <c r="HW7" s="3"/>
+      <c r="HX7" s="3"/>
+      <c r="HY7" s="3"/>
+      <c r="HZ7" s="3"/>
+      <c r="IA7" s="3"/>
+      <c r="IB7" s="3"/>
+      <c r="IC7" s="3"/>
+      <c r="ID7" s="3"/>
+      <c r="IE7" s="3"/>
+      <c r="IF7" s="3"/>
+      <c r="IG7" s="3"/>
+      <c r="IH7" s="3"/>
+      <c r="II7" s="3"/>
+      <c r="IJ7" s="3"/>
+      <c r="IK7" s="3"/>
+      <c r="IL7" s="3"/>
+      <c r="IM7" s="3"/>
+      <c r="IN7" s="3"/>
+      <c r="IO7" s="3"/>
+      <c r="IP7" s="3"/>
+      <c r="IQ7" s="3"/>
+      <c r="IR7" s="3"/>
+      <c r="IS7" s="3"/>
+      <c r="IT7" s="3"/>
+      <c r="IU7" s="3"/>
+      <c r="IV7" s="3"/>
     </row>
     <row r="8" spans="1:256" ht="13.5">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>khan2012.py</t>
+          <t>"Normalised to data size"?</t>
         </is>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>Single column? </t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="4"/>
-      <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="4"/>
-      <c r="AF8" s="4"/>
-      <c r="AG8" s="4"/>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="4"/>
-      <c r="AJ8" s="4"/>
-      <c r="AK8" s="4"/>
-      <c r="AL8" s="4"/>
-      <c r="AM8" s="4"/>
-      <c r="AN8" s="4"/>
-      <c r="AO8" s="4"/>
-      <c r="AP8" s="4"/>
-      <c r="AQ8" s="4"/>
-      <c r="AR8" s="4"/>
-      <c r="AS8" s="4"/>
-      <c r="AT8" s="4"/>
-      <c r="AU8" s="4"/>
-      <c r="AV8" s="4"/>
-      <c r="AW8" s="4"/>
-      <c r="AX8" s="4"/>
-      <c r="AY8" s="4"/>
-      <c r="AZ8" s="4"/>
-      <c r="BA8" s="4"/>
-      <c r="BB8" s="4"/>
-      <c r="BC8" s="4"/>
-      <c r="BD8" s="4"/>
-      <c r="BE8" s="4"/>
-      <c r="BF8" s="4"/>
-      <c r="BG8" s="4"/>
-      <c r="BH8" s="4"/>
-      <c r="BI8" s="4"/>
-      <c r="BJ8" s="4"/>
-      <c r="BK8" s="4"/>
-      <c r="BL8" s="4"/>
-      <c r="BM8" s="4"/>
-      <c r="BN8" s="4"/>
-      <c r="BO8" s="4"/>
-      <c r="BP8" s="4"/>
-      <c r="BQ8" s="4"/>
-      <c r="BR8" s="4"/>
-      <c r="BS8" s="4"/>
-      <c r="BT8" s="4"/>
-      <c r="BU8" s="4"/>
-      <c r="BV8" s="4"/>
-      <c r="BW8" s="4"/>
-      <c r="BX8" s="4"/>
-      <c r="BY8" s="4"/>
-      <c r="BZ8" s="4"/>
-      <c r="CA8" s="4"/>
-      <c r="CB8" s="4"/>
-      <c r="CC8" s="4"/>
-      <c r="CD8" s="4"/>
-      <c r="CE8" s="4"/>
-      <c r="CF8" s="4"/>
-      <c r="CG8" s="4"/>
-      <c r="CH8" s="4"/>
-      <c r="CI8" s="4"/>
-      <c r="CJ8" s="4"/>
-      <c r="CK8" s="4"/>
-      <c r="CL8" s="4"/>
-      <c r="CM8" s="4"/>
-      <c r="CN8" s="4"/>
-      <c r="CO8" s="4"/>
-      <c r="CP8" s="4"/>
-      <c r="CQ8" s="4"/>
-      <c r="CR8" s="4"/>
-      <c r="CS8" s="4"/>
-      <c r="CT8" s="4"/>
-      <c r="CU8" s="4"/>
-      <c r="CV8" s="4"/>
-      <c r="CW8" s="4"/>
-      <c r="CX8" s="4"/>
-      <c r="CY8" s="4"/>
-      <c r="CZ8" s="4"/>
-      <c r="DA8" s="4"/>
-      <c r="DB8" s="4"/>
-      <c r="DC8" s="4"/>
-      <c r="DD8" s="4"/>
-      <c r="DE8" s="4"/>
-      <c r="DF8" s="4"/>
-      <c r="DG8" s="4"/>
-      <c r="DH8" s="4"/>
-      <c r="DI8" s="4"/>
-      <c r="DJ8" s="4"/>
-      <c r="DK8" s="4"/>
-      <c r="DL8" s="4"/>
-      <c r="DM8" s="4"/>
-      <c r="DN8" s="4"/>
-      <c r="DO8" s="4"/>
-      <c r="DP8" s="4"/>
-      <c r="DQ8" s="4"/>
-      <c r="DR8" s="4"/>
-      <c r="DS8" s="4"/>
-      <c r="DT8" s="4"/>
-      <c r="DU8" s="4"/>
-      <c r="DV8" s="4"/>
-      <c r="DW8" s="4"/>
-      <c r="DX8" s="4"/>
-      <c r="DY8" s="4"/>
-      <c r="DZ8" s="4"/>
-      <c r="EA8" s="4"/>
-      <c r="EB8" s="4"/>
-      <c r="EC8" s="4"/>
-      <c r="ED8" s="4"/>
-      <c r="EE8" s="4"/>
-      <c r="EF8" s="4"/>
-      <c r="EG8" s="4"/>
-      <c r="EH8" s="4"/>
-      <c r="EI8" s="4"/>
-      <c r="EJ8" s="4"/>
-      <c r="EK8" s="4"/>
-      <c r="EL8" s="4"/>
-      <c r="EM8" s="4"/>
-      <c r="EN8" s="4"/>
-      <c r="EO8" s="4"/>
-      <c r="EP8" s="4"/>
-      <c r="EQ8" s="4"/>
-      <c r="ER8" s="4"/>
-      <c r="ES8" s="4"/>
-      <c r="ET8" s="4"/>
-      <c r="EU8" s="4"/>
-      <c r="EV8" s="4"/>
-      <c r="EW8" s="4"/>
-      <c r="EX8" s="4"/>
-      <c r="EY8" s="4"/>
-      <c r="EZ8" s="4"/>
-      <c r="FA8" s="4"/>
-      <c r="FB8" s="4"/>
-      <c r="FC8" s="4"/>
-      <c r="FD8" s="4"/>
-      <c r="FE8" s="4"/>
-      <c r="FF8" s="4"/>
-      <c r="FG8" s="4"/>
-      <c r="FH8" s="4"/>
-      <c r="FI8" s="4"/>
-      <c r="FJ8" s="4"/>
-      <c r="FK8" s="4"/>
-      <c r="FL8" s="4"/>
-      <c r="FM8" s="4"/>
-      <c r="FN8" s="4"/>
-      <c r="FO8" s="4"/>
-      <c r="FP8" s="4"/>
-      <c r="FQ8" s="4"/>
-      <c r="FR8" s="4"/>
-      <c r="FS8" s="4"/>
-      <c r="FT8" s="4"/>
-      <c r="FU8" s="4"/>
-      <c r="FV8" s="4"/>
-      <c r="FW8" s="4"/>
-      <c r="FX8" s="4"/>
-      <c r="FY8" s="4"/>
-      <c r="FZ8" s="4"/>
-      <c r="GA8" s="4"/>
-      <c r="GB8" s="4"/>
-      <c r="GC8" s="4"/>
-      <c r="GD8" s="4"/>
-      <c r="GE8" s="4"/>
-      <c r="GF8" s="4"/>
-      <c r="GG8" s="4"/>
-      <c r="GH8" s="4"/>
-      <c r="GI8" s="4"/>
-      <c r="GJ8" s="4"/>
-      <c r="GK8" s="4"/>
-      <c r="GL8" s="4"/>
-      <c r="GM8" s="4"/>
-      <c r="GN8" s="4"/>
-      <c r="GO8" s="4"/>
-      <c r="GP8" s="4"/>
-      <c r="GQ8" s="4"/>
-      <c r="GR8" s="4"/>
-      <c r="GS8" s="4"/>
-      <c r="GT8" s="4"/>
-      <c r="GU8" s="4"/>
-      <c r="GV8" s="4"/>
-      <c r="GW8" s="4"/>
-      <c r="GX8" s="4"/>
-      <c r="GY8" s="4"/>
-      <c r="GZ8" s="4"/>
-      <c r="HA8" s="4"/>
-      <c r="HB8" s="4"/>
-      <c r="HC8" s="4"/>
-      <c r="HD8" s="4"/>
-      <c r="HE8" s="4"/>
-      <c r="HF8" s="4"/>
-      <c r="HG8" s="4"/>
-      <c r="HH8" s="4"/>
-      <c r="HI8" s="4"/>
-      <c r="HJ8" s="4"/>
-      <c r="HK8" s="4"/>
-      <c r="HL8" s="4"/>
-      <c r="HM8" s="4"/>
-      <c r="HN8" s="4"/>
-      <c r="HO8" s="4"/>
-      <c r="HP8" s="4"/>
-      <c r="HQ8" s="4"/>
-      <c r="HR8" s="4"/>
-      <c r="HS8" s="4"/>
-      <c r="HT8" s="4"/>
-      <c r="HU8" s="4"/>
-      <c r="HV8" s="4"/>
-      <c r="HW8" s="4"/>
-      <c r="HX8" s="4"/>
-      <c r="HY8" s="4"/>
-      <c r="HZ8" s="4"/>
-      <c r="IA8" s="4"/>
-      <c r="IB8" s="4"/>
-      <c r="IC8" s="4"/>
-      <c r="ID8" s="4"/>
-      <c r="IE8" s="4"/>
-      <c r="IF8" s="4"/>
-      <c r="IG8" s="4"/>
-      <c r="IH8" s="4"/>
-      <c r="II8" s="4"/>
-      <c r="IJ8" s="4"/>
-      <c r="IK8" s="4"/>
-      <c r="IL8" s="4"/>
-      <c r="IM8" s="4"/>
-      <c r="IN8" s="4"/>
-      <c r="IO8" s="4"/>
-      <c r="IP8" s="4"/>
-      <c r="IQ8" s="4"/>
-      <c r="IR8" s="4"/>
-      <c r="IS8" s="4"/>
-      <c r="IT8" s="4"/>
-      <c r="IU8" s="4"/>
-      <c r="IV8" s="4"/>
+      <c r="G8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
+      <c r="AT8" s="3"/>
+      <c r="AU8" s="3"/>
+      <c r="AV8" s="3"/>
+      <c r="AW8" s="3"/>
+      <c r="AX8" s="3"/>
+      <c r="AY8" s="3"/>
+      <c r="AZ8" s="3"/>
+      <c r="BA8" s="3"/>
+      <c r="BB8" s="3"/>
+      <c r="BC8" s="3"/>
+      <c r="BD8" s="3"/>
+      <c r="BE8" s="3"/>
+      <c r="BF8" s="3"/>
+      <c r="BG8" s="3"/>
+      <c r="BH8" s="3"/>
+      <c r="BI8" s="3"/>
+      <c r="BJ8" s="3"/>
+      <c r="BK8" s="3"/>
+      <c r="BL8" s="3"/>
+      <c r="BM8" s="3"/>
+      <c r="BN8" s="3"/>
+      <c r="BO8" s="3"/>
+      <c r="BP8" s="3"/>
+      <c r="BQ8" s="3"/>
+      <c r="BR8" s="3"/>
+      <c r="BS8" s="3"/>
+      <c r="BT8" s="3"/>
+      <c r="BU8" s="3"/>
+      <c r="BV8" s="3"/>
+      <c r="BW8" s="3"/>
+      <c r="BX8" s="3"/>
+      <c r="BY8" s="3"/>
+      <c r="BZ8" s="3"/>
+      <c r="CA8" s="3"/>
+      <c r="CB8" s="3"/>
+      <c r="CC8" s="3"/>
+      <c r="CD8" s="3"/>
+      <c r="CE8" s="3"/>
+      <c r="CF8" s="3"/>
+      <c r="CG8" s="3"/>
+      <c r="CH8" s="3"/>
+      <c r="CI8" s="3"/>
+      <c r="CJ8" s="3"/>
+      <c r="CK8" s="3"/>
+      <c r="CL8" s="3"/>
+      <c r="CM8" s="3"/>
+      <c r="CN8" s="3"/>
+      <c r="CO8" s="3"/>
+      <c r="CP8" s="3"/>
+      <c r="CQ8" s="3"/>
+      <c r="CR8" s="3"/>
+      <c r="CS8" s="3"/>
+      <c r="CT8" s="3"/>
+      <c r="CU8" s="3"/>
+      <c r="CV8" s="3"/>
+      <c r="CW8" s="3"/>
+      <c r="CX8" s="3"/>
+      <c r="CY8" s="3"/>
+      <c r="CZ8" s="3"/>
+      <c r="DA8" s="3"/>
+      <c r="DB8" s="3"/>
+      <c r="DC8" s="3"/>
+      <c r="DD8" s="3"/>
+      <c r="DE8" s="3"/>
+      <c r="DF8" s="3"/>
+      <c r="DG8" s="3"/>
+      <c r="DH8" s="3"/>
+      <c r="DI8" s="3"/>
+      <c r="DJ8" s="3"/>
+      <c r="DK8" s="3"/>
+      <c r="DL8" s="3"/>
+      <c r="DM8" s="3"/>
+      <c r="DN8" s="3"/>
+      <c r="DO8" s="3"/>
+      <c r="DP8" s="3"/>
+      <c r="DQ8" s="3"/>
+      <c r="DR8" s="3"/>
+      <c r="DS8" s="3"/>
+      <c r="DT8" s="3"/>
+      <c r="DU8" s="3"/>
+      <c r="DV8" s="3"/>
+      <c r="DW8" s="3"/>
+      <c r="DX8" s="3"/>
+      <c r="DY8" s="3"/>
+      <c r="DZ8" s="3"/>
+      <c r="EA8" s="3"/>
+      <c r="EB8" s="3"/>
+      <c r="EC8" s="3"/>
+      <c r="ED8" s="3"/>
+      <c r="EE8" s="3"/>
+      <c r="EF8" s="3"/>
+      <c r="EG8" s="3"/>
+      <c r="EH8" s="3"/>
+      <c r="EI8" s="3"/>
+      <c r="EJ8" s="3"/>
+      <c r="EK8" s="3"/>
+      <c r="EL8" s="3"/>
+      <c r="EM8" s="3"/>
+      <c r="EN8" s="3"/>
+      <c r="EO8" s="3"/>
+      <c r="EP8" s="3"/>
+      <c r="EQ8" s="3"/>
+      <c r="ER8" s="3"/>
+      <c r="ES8" s="3"/>
+      <c r="ET8" s="3"/>
+      <c r="EU8" s="3"/>
+      <c r="EV8" s="3"/>
+      <c r="EW8" s="3"/>
+      <c r="EX8" s="3"/>
+      <c r="EY8" s="3"/>
+      <c r="EZ8" s="3"/>
+      <c r="FA8" s="3"/>
+      <c r="FB8" s="3"/>
+      <c r="FC8" s="3"/>
+      <c r="FD8" s="3"/>
+      <c r="FE8" s="3"/>
+      <c r="FF8" s="3"/>
+      <c r="FG8" s="3"/>
+      <c r="FH8" s="3"/>
+      <c r="FI8" s="3"/>
+      <c r="FJ8" s="3"/>
+      <c r="FK8" s="3"/>
+      <c r="FL8" s="3"/>
+      <c r="FM8" s="3"/>
+      <c r="FN8" s="3"/>
+      <c r="FO8" s="3"/>
+      <c r="FP8" s="3"/>
+      <c r="FQ8" s="3"/>
+      <c r="FR8" s="3"/>
+      <c r="FS8" s="3"/>
+      <c r="FT8" s="3"/>
+      <c r="FU8" s="3"/>
+      <c r="FV8" s="3"/>
+      <c r="FW8" s="3"/>
+      <c r="FX8" s="3"/>
+      <c r="FY8" s="3"/>
+      <c r="FZ8" s="3"/>
+      <c r="GA8" s="3"/>
+      <c r="GB8" s="3"/>
+      <c r="GC8" s="3"/>
+      <c r="GD8" s="3"/>
+      <c r="GE8" s="3"/>
+      <c r="GF8" s="3"/>
+      <c r="GG8" s="3"/>
+      <c r="GH8" s="3"/>
+      <c r="GI8" s="3"/>
+      <c r="GJ8" s="3"/>
+      <c r="GK8" s="3"/>
+      <c r="GL8" s="3"/>
+      <c r="GM8" s="3"/>
+      <c r="GN8" s="3"/>
+      <c r="GO8" s="3"/>
+      <c r="GP8" s="3"/>
+      <c r="GQ8" s="3"/>
+      <c r="GR8" s="3"/>
+      <c r="GS8" s="3"/>
+      <c r="GT8" s="3"/>
+      <c r="GU8" s="3"/>
+      <c r="GV8" s="3"/>
+      <c r="GW8" s="3"/>
+      <c r="GX8" s="3"/>
+      <c r="GY8" s="3"/>
+      <c r="GZ8" s="3"/>
+      <c r="HA8" s="3"/>
+      <c r="HB8" s="3"/>
+      <c r="HC8" s="3"/>
+      <c r="HD8" s="3"/>
+      <c r="HE8" s="3"/>
+      <c r="HF8" s="3"/>
+      <c r="HG8" s="3"/>
+      <c r="HH8" s="3"/>
+      <c r="HI8" s="3"/>
+      <c r="HJ8" s="3"/>
+      <c r="HK8" s="3"/>
+      <c r="HL8" s="3"/>
+      <c r="HM8" s="3"/>
+      <c r="HN8" s="3"/>
+      <c r="HO8" s="3"/>
+      <c r="HP8" s="3"/>
+      <c r="HQ8" s="3"/>
+      <c r="HR8" s="3"/>
+      <c r="HS8" s="3"/>
+      <c r="HT8" s="3"/>
+      <c r="HU8" s="3"/>
+      <c r="HV8" s="3"/>
+      <c r="HW8" s="3"/>
+      <c r="HX8" s="3"/>
+      <c r="HY8" s="3"/>
+      <c r="HZ8" s="3"/>
+      <c r="IA8" s="3"/>
+      <c r="IB8" s="3"/>
+      <c r="IC8" s="3"/>
+      <c r="ID8" s="3"/>
+      <c r="IE8" s="3"/>
+      <c r="IF8" s="3"/>
+      <c r="IG8" s="3"/>
+      <c r="IH8" s="3"/>
+      <c r="II8" s="3"/>
+      <c r="IJ8" s="3"/>
+      <c r="IK8" s="3"/>
+      <c r="IL8" s="3"/>
+      <c r="IM8" s="3"/>
+      <c r="IN8" s="3"/>
+      <c r="IO8" s="3"/>
+      <c r="IP8" s="3"/>
+      <c r="IQ8" s="3"/>
+      <c r="IR8" s="3"/>
+      <c r="IS8" s="3"/>
+      <c r="IT8" s="3"/>
+      <c r="IU8" s="3"/>
+      <c r="IV8" s="3"/>
     </row>
     <row r="9" spans="1:256" ht="13.5">
       <c r="A9" t="inlineStr">
@@ -2155,13 +2429,13 @@
         </is>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:256" ht="13.5">
@@ -3005,8 +3279,10 @@
       <c r="IV12" s="3"/>
     </row>
     <row r="13" spans="1:256" ht="13.5">
-      <c r="A13" s="3" t="s">
-        <v>6</v>
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>macqueen1967.py</t>
+        </is>
       </c>
       <c r="B13" s="3" t="s">
         <v>0</v>
@@ -3014,17 +3290,15 @@
       <c r="C13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="3" t="inlineStr">
-        <is>
-          <t>ro</t>
-        </is>
+      <c r="D13" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>Not given: "reported elsewhere"?</t>
+          <t>Not given; "To be published elsewhere"</t>
         </is>
       </c>
       <c r="G13" s="3" t="s">
@@ -3032,12 +3306,12 @@
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>Y - BROKEN</t>
+          <t>Y; broken</t>
         </is>
       </c>
       <c r="I13" s="3" t="inlineStr">
         <is>
-          <t>~ Except R/C issues</t>
+          <t>~; Except R&amp;C</t>
         </is>
       </c>
       <c r="J13" s="3"/>
@@ -3300,7 +3574,7 @@
       <c r="C14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -3578,8 +3852,8 @@
       <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
-        <v>1</v>
+      <c r="D15" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>4</v>
@@ -3858,8 +4132,8 @@
       <c r="C16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D16" t="s">
-        <v>1</v>
+      <c r="D16" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>4</v>
@@ -4138,7 +4412,7 @@
       <c r="C17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -4416,8 +4690,8 @@
       <c r="C18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D18" t="s">
-        <v>1</v>
+      <c r="D18" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>2</v>
@@ -4696,7 +4970,7 @@
       <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -4966,539 +5240,1571 @@
     </row>
     <row r="20" spans="1:256" ht="13.5"/>
     <row r="21" spans="1:256" ht="13.5"/>
-    <row r="24" spans="1:256">
-      <c r="A24" s="5" t="inlineStr">
+    <row r="22" spans="1:256">
+      <c r="A22" s="4" t="inlineStr">
         <is>
           <t>steinley2007.py</t>
         </is>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5" t="inlineStr">
+      <c r="B22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-      <c r="Z24" s="5"/>
-      <c r="AA24" s="5"/>
-      <c r="AB24" s="5"/>
-      <c r="AC24" s="5"/>
-      <c r="AD24" s="5"/>
-      <c r="AE24" s="5"/>
-      <c r="AF24" s="5"/>
-      <c r="AG24" s="5"/>
-      <c r="AH24" s="5"/>
-      <c r="AI24" s="5"/>
-      <c r="AJ24" s="5"/>
-      <c r="AK24" s="5"/>
-      <c r="AL24" s="5"/>
-      <c r="AM24" s="5"/>
-      <c r="AN24" s="5"/>
-      <c r="AO24" s="5"/>
-      <c r="AP24" s="5"/>
-      <c r="AQ24" s="5"/>
-      <c r="AR24" s="5"/>
-      <c r="AS24" s="5"/>
-      <c r="AT24" s="5"/>
-      <c r="AU24" s="5"/>
-      <c r="AV24" s="5"/>
-      <c r="AW24" s="5"/>
-      <c r="AX24" s="5"/>
-      <c r="AY24" s="5"/>
-      <c r="AZ24" s="5"/>
-      <c r="BA24" s="5"/>
-      <c r="BB24" s="5"/>
-      <c r="BC24" s="5"/>
-      <c r="BD24" s="5"/>
-      <c r="BE24" s="5"/>
-      <c r="BF24" s="5"/>
-      <c r="BG24" s="5"/>
-      <c r="BH24" s="5"/>
-      <c r="BI24" s="5"/>
-      <c r="BJ24" s="5"/>
-      <c r="BK24" s="5"/>
-      <c r="BL24" s="5"/>
-      <c r="BM24" s="5"/>
-      <c r="BN24" s="5"/>
-      <c r="BO24" s="5"/>
-      <c r="BP24" s="5"/>
-      <c r="BQ24" s="5"/>
-      <c r="BR24" s="5"/>
-      <c r="BS24" s="5"/>
-      <c r="BT24" s="5"/>
-      <c r="BU24" s="5"/>
-      <c r="BV24" s="5"/>
-      <c r="BW24" s="5"/>
-      <c r="BX24" s="5"/>
-      <c r="BY24" s="5"/>
-      <c r="BZ24" s="5"/>
-      <c r="CA24" s="5"/>
-      <c r="CB24" s="5"/>
-      <c r="CC24" s="5"/>
-      <c r="CD24" s="5"/>
-      <c r="CE24" s="5"/>
-      <c r="CF24" s="5"/>
-      <c r="CG24" s="5"/>
-      <c r="CH24" s="5"/>
-      <c r="CI24" s="5"/>
-      <c r="CJ24" s="5"/>
-      <c r="CK24" s="5"/>
-      <c r="CL24" s="5"/>
-      <c r="CM24" s="5"/>
-      <c r="CN24" s="5"/>
-      <c r="CO24" s="5"/>
-      <c r="CP24" s="5"/>
-      <c r="CQ24" s="5"/>
-      <c r="CR24" s="5"/>
-      <c r="CS24" s="5"/>
-      <c r="CT24" s="5"/>
-      <c r="CU24" s="5"/>
-      <c r="CV24" s="5"/>
-      <c r="CW24" s="5"/>
-      <c r="CX24" s="5"/>
-      <c r="CY24" s="5"/>
-      <c r="CZ24" s="5"/>
-      <c r="DA24" s="5"/>
-      <c r="DB24" s="5"/>
-      <c r="DC24" s="5"/>
-      <c r="DD24" s="5"/>
-      <c r="DE24" s="5"/>
-      <c r="DF24" s="5"/>
-      <c r="DG24" s="5"/>
-      <c r="DH24" s="5"/>
-      <c r="DI24" s="5"/>
-      <c r="DJ24" s="5"/>
-      <c r="DK24" s="5"/>
-      <c r="DL24" s="5"/>
-      <c r="DM24" s="5"/>
-      <c r="DN24" s="5"/>
-      <c r="DO24" s="5"/>
-      <c r="DP24" s="5"/>
-      <c r="DQ24" s="5"/>
-      <c r="DR24" s="5"/>
-      <c r="DS24" s="5"/>
-      <c r="DT24" s="5"/>
-      <c r="DU24" s="5"/>
-      <c r="DV24" s="5"/>
-      <c r="DW24" s="5"/>
-      <c r="DX24" s="5"/>
-      <c r="DY24" s="5"/>
-      <c r="DZ24" s="5"/>
-      <c r="EA24" s="5"/>
-      <c r="EB24" s="5"/>
-      <c r="EC24" s="5"/>
-      <c r="ED24" s="5"/>
-      <c r="EE24" s="5"/>
-      <c r="EF24" s="5"/>
-      <c r="EG24" s="5"/>
-      <c r="EH24" s="5"/>
-      <c r="EI24" s="5"/>
-      <c r="EJ24" s="5"/>
-      <c r="EK24" s="5"/>
-      <c r="EL24" s="5"/>
-      <c r="EM24" s="5"/>
-      <c r="EN24" s="5"/>
-      <c r="EO24" s="5"/>
-      <c r="EP24" s="5"/>
-      <c r="EQ24" s="5"/>
-      <c r="ER24" s="5"/>
-      <c r="ES24" s="5"/>
-      <c r="ET24" s="5"/>
-      <c r="EU24" s="5"/>
-      <c r="EV24" s="5"/>
-      <c r="EW24" s="5"/>
-      <c r="EX24" s="5"/>
-      <c r="EY24" s="5"/>
-      <c r="EZ24" s="5"/>
-      <c r="FA24" s="5"/>
-      <c r="FB24" s="5"/>
-      <c r="FC24" s="5"/>
-      <c r="FD24" s="5"/>
-      <c r="FE24" s="5"/>
-      <c r="FF24" s="5"/>
-      <c r="FG24" s="5"/>
-      <c r="FH24" s="5"/>
-      <c r="FI24" s="5"/>
-      <c r="FJ24" s="5"/>
-      <c r="FK24" s="5"/>
-      <c r="FL24" s="5"/>
-      <c r="FM24" s="5"/>
-      <c r="FN24" s="5"/>
-      <c r="FO24" s="5"/>
-      <c r="FP24" s="5"/>
-      <c r="FQ24" s="5"/>
-      <c r="FR24" s="5"/>
-      <c r="FS24" s="5"/>
-      <c r="FT24" s="5"/>
-      <c r="FU24" s="5"/>
-      <c r="FV24" s="5"/>
-      <c r="FW24" s="5"/>
-      <c r="FX24" s="5"/>
-      <c r="FY24" s="5"/>
-      <c r="FZ24" s="5"/>
-      <c r="GA24" s="5"/>
-      <c r="GB24" s="5"/>
-      <c r="GC24" s="5"/>
-      <c r="GD24" s="5"/>
-      <c r="GE24" s="5"/>
-      <c r="GF24" s="5"/>
-      <c r="GG24" s="5"/>
-      <c r="GH24" s="5"/>
-      <c r="GI24" s="5"/>
-      <c r="GJ24" s="5"/>
-      <c r="GK24" s="5"/>
-      <c r="GL24" s="5"/>
-      <c r="GM24" s="5"/>
-      <c r="GN24" s="5"/>
-      <c r="GO24" s="5"/>
-      <c r="GP24" s="5"/>
-      <c r="GQ24" s="5"/>
-      <c r="GR24" s="5"/>
-      <c r="GS24" s="5"/>
-      <c r="GT24" s="5"/>
-      <c r="GU24" s="5"/>
-      <c r="GV24" s="5"/>
-      <c r="GW24" s="5"/>
-      <c r="GX24" s="5"/>
-      <c r="GY24" s="5"/>
-      <c r="GZ24" s="5"/>
-      <c r="HA24" s="5"/>
-      <c r="HB24" s="5"/>
-      <c r="HC24" s="5"/>
-      <c r="HD24" s="5"/>
-      <c r="HE24" s="5"/>
-      <c r="HF24" s="5"/>
-      <c r="HG24" s="5"/>
-      <c r="HH24" s="5"/>
-      <c r="HI24" s="5"/>
-      <c r="HJ24" s="5"/>
-      <c r="HK24" s="5"/>
-      <c r="HL24" s="5"/>
-      <c r="HM24" s="5"/>
-      <c r="HN24" s="5"/>
-      <c r="HO24" s="5"/>
-      <c r="HP24" s="5"/>
-      <c r="HQ24" s="5"/>
-      <c r="HR24" s="5"/>
-      <c r="HS24" s="5"/>
-      <c r="HT24" s="5"/>
-      <c r="HU24" s="5"/>
-      <c r="HV24" s="5"/>
-      <c r="HW24" s="5"/>
-      <c r="HX24" s="5"/>
-      <c r="HY24" s="5"/>
-      <c r="HZ24" s="5"/>
-      <c r="IA24" s="5"/>
-      <c r="IB24" s="5"/>
-      <c r="IC24" s="5"/>
-      <c r="ID24" s="5"/>
-      <c r="IE24" s="5"/>
-      <c r="IF24" s="5"/>
-      <c r="IG24" s="5"/>
-      <c r="IH24" s="5"/>
-      <c r="II24" s="5"/>
-      <c r="IJ24" s="5"/>
-      <c r="IK24" s="5"/>
-      <c r="IL24" s="5"/>
-      <c r="IM24" s="5"/>
-      <c r="IN24" s="5"/>
-      <c r="IO24" s="5"/>
-      <c r="IP24" s="5"/>
-      <c r="IQ24" s="5"/>
-      <c r="IR24" s="5"/>
-      <c r="IS24" s="5"/>
-      <c r="IT24" s="5"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="4"/>
+      <c r="AJ22" s="4"/>
+      <c r="AK22" s="4"/>
+      <c r="AL22" s="4"/>
+      <c r="AM22" s="4"/>
+      <c r="AN22" s="4"/>
+      <c r="AO22" s="4"/>
+      <c r="AP22" s="4"/>
+      <c r="AQ22" s="4"/>
+      <c r="AR22" s="4"/>
+      <c r="AS22" s="4"/>
+      <c r="AT22" s="4"/>
+      <c r="AU22" s="4"/>
+      <c r="AV22" s="4"/>
+      <c r="AW22" s="4"/>
+      <c r="AX22" s="4"/>
+      <c r="AY22" s="4"/>
+      <c r="AZ22" s="4"/>
+      <c r="BA22" s="4"/>
+      <c r="BB22" s="4"/>
+      <c r="BC22" s="4"/>
+      <c r="BD22" s="4"/>
+      <c r="BE22" s="4"/>
+      <c r="BF22" s="4"/>
+      <c r="BG22" s="4"/>
+      <c r="BH22" s="4"/>
+      <c r="BI22" s="4"/>
+      <c r="BJ22" s="4"/>
+      <c r="BK22" s="4"/>
+      <c r="BL22" s="4"/>
+      <c r="BM22" s="4"/>
+      <c r="BN22" s="4"/>
+      <c r="BO22" s="4"/>
+      <c r="BP22" s="4"/>
+      <c r="BQ22" s="4"/>
+      <c r="BR22" s="4"/>
+      <c r="BS22" s="4"/>
+      <c r="BT22" s="4"/>
+      <c r="BU22" s="4"/>
+      <c r="BV22" s="4"/>
+      <c r="BW22" s="4"/>
+      <c r="BX22" s="4"/>
+      <c r="BY22" s="4"/>
+      <c r="BZ22" s="4"/>
+      <c r="CA22" s="4"/>
+      <c r="CB22" s="4"/>
+      <c r="CC22" s="4"/>
+      <c r="CD22" s="4"/>
+      <c r="CE22" s="4"/>
+      <c r="CF22" s="4"/>
+      <c r="CG22" s="4"/>
+      <c r="CH22" s="4"/>
+      <c r="CI22" s="4"/>
+      <c r="CJ22" s="4"/>
+      <c r="CK22" s="4"/>
+      <c r="CL22" s="4"/>
+      <c r="CM22" s="4"/>
+      <c r="CN22" s="4"/>
+      <c r="CO22" s="4"/>
+      <c r="CP22" s="4"/>
+      <c r="CQ22" s="4"/>
+      <c r="CR22" s="4"/>
+      <c r="CS22" s="4"/>
+      <c r="CT22" s="4"/>
+      <c r="CU22" s="4"/>
+      <c r="CV22" s="4"/>
+      <c r="CW22" s="4"/>
+      <c r="CX22" s="4"/>
+      <c r="CY22" s="4"/>
+      <c r="CZ22" s="4"/>
+      <c r="DA22" s="4"/>
+      <c r="DB22" s="4"/>
+      <c r="DC22" s="4"/>
+      <c r="DD22" s="4"/>
+      <c r="DE22" s="4"/>
+      <c r="DF22" s="4"/>
+      <c r="DG22" s="4"/>
+      <c r="DH22" s="4"/>
+      <c r="DI22" s="4"/>
+      <c r="DJ22" s="4"/>
+      <c r="DK22" s="4"/>
+      <c r="DL22" s="4"/>
+      <c r="DM22" s="4"/>
+      <c r="DN22" s="4"/>
+      <c r="DO22" s="4"/>
+      <c r="DP22" s="4"/>
+      <c r="DQ22" s="4"/>
+      <c r="DR22" s="4"/>
+      <c r="DS22" s="4"/>
+      <c r="DT22" s="4"/>
+      <c r="DU22" s="4"/>
+      <c r="DV22" s="4"/>
+      <c r="DW22" s="4"/>
+      <c r="DX22" s="4"/>
+      <c r="DY22" s="4"/>
+      <c r="DZ22" s="4"/>
+      <c r="EA22" s="4"/>
+      <c r="EB22" s="4"/>
+      <c r="EC22" s="4"/>
+      <c r="ED22" s="4"/>
+      <c r="EE22" s="4"/>
+      <c r="EF22" s="4"/>
+      <c r="EG22" s="4"/>
+      <c r="EH22" s="4"/>
+      <c r="EI22" s="4"/>
+      <c r="EJ22" s="4"/>
+      <c r="EK22" s="4"/>
+      <c r="EL22" s="4"/>
+      <c r="EM22" s="4"/>
+      <c r="EN22" s="4"/>
+      <c r="EO22" s="4"/>
+      <c r="EP22" s="4"/>
+      <c r="EQ22" s="4"/>
+      <c r="ER22" s="4"/>
+      <c r="ES22" s="4"/>
+      <c r="ET22" s="4"/>
+      <c r="EU22" s="4"/>
+      <c r="EV22" s="4"/>
+      <c r="EW22" s="4"/>
+      <c r="EX22" s="4"/>
+      <c r="EY22" s="4"/>
+      <c r="EZ22" s="4"/>
+      <c r="FA22" s="4"/>
+      <c r="FB22" s="4"/>
+      <c r="FC22" s="4"/>
+      <c r="FD22" s="4"/>
+      <c r="FE22" s="4"/>
+      <c r="FF22" s="4"/>
+      <c r="FG22" s="4"/>
+      <c r="FH22" s="4"/>
+      <c r="FI22" s="4"/>
+      <c r="FJ22" s="4"/>
+      <c r="FK22" s="4"/>
+      <c r="FL22" s="4"/>
+      <c r="FM22" s="4"/>
+      <c r="FN22" s="4"/>
+      <c r="FO22" s="4"/>
+      <c r="FP22" s="4"/>
+      <c r="FQ22" s="4"/>
+      <c r="FR22" s="4"/>
+      <c r="FS22" s="4"/>
+      <c r="FT22" s="4"/>
+      <c r="FU22" s="4"/>
+      <c r="FV22" s="4"/>
+      <c r="FW22" s="4"/>
+      <c r="FX22" s="4"/>
+      <c r="FY22" s="4"/>
+      <c r="FZ22" s="4"/>
+      <c r="GA22" s="4"/>
+      <c r="GB22" s="4"/>
+      <c r="GC22" s="4"/>
+      <c r="GD22" s="4"/>
+      <c r="GE22" s="4"/>
+      <c r="GF22" s="4"/>
+      <c r="GG22" s="4"/>
+      <c r="GH22" s="4"/>
+      <c r="GI22" s="4"/>
+      <c r="GJ22" s="4"/>
+      <c r="GK22" s="4"/>
+      <c r="GL22" s="4"/>
+      <c r="GM22" s="4"/>
+      <c r="GN22" s="4"/>
+      <c r="GO22" s="4"/>
+      <c r="GP22" s="4"/>
+      <c r="GQ22" s="4"/>
+      <c r="GR22" s="4"/>
+      <c r="GS22" s="4"/>
+      <c r="GT22" s="4"/>
+      <c r="GU22" s="4"/>
+      <c r="GV22" s="4"/>
+      <c r="GW22" s="4"/>
+      <c r="GX22" s="4"/>
+      <c r="GY22" s="4"/>
+      <c r="GZ22" s="4"/>
+      <c r="HA22" s="4"/>
+      <c r="HB22" s="4"/>
+      <c r="HC22" s="4"/>
+      <c r="HD22" s="4"/>
+      <c r="HE22" s="4"/>
+      <c r="HF22" s="4"/>
+      <c r="HG22" s="4"/>
+      <c r="HH22" s="4"/>
+      <c r="HI22" s="4"/>
+      <c r="HJ22" s="4"/>
+      <c r="HK22" s="4"/>
+      <c r="HL22" s="4"/>
+      <c r="HM22" s="4"/>
+      <c r="HN22" s="4"/>
+      <c r="HO22" s="4"/>
+      <c r="HP22" s="4"/>
+      <c r="HQ22" s="4"/>
+      <c r="HR22" s="4"/>
+      <c r="HS22" s="4"/>
+      <c r="HT22" s="4"/>
+      <c r="HU22" s="4"/>
+      <c r="HV22" s="4"/>
+      <c r="HW22" s="4"/>
+      <c r="HX22" s="4"/>
+      <c r="HY22" s="4"/>
+      <c r="HZ22" s="4"/>
+      <c r="IA22" s="4"/>
+      <c r="IB22" s="4"/>
+      <c r="IC22" s="4"/>
+      <c r="ID22" s="4"/>
+      <c r="IE22" s="4"/>
+      <c r="IF22" s="4"/>
+      <c r="IG22" s="4"/>
+      <c r="IH22" s="4"/>
+      <c r="II22" s="4"/>
+      <c r="IJ22" s="4"/>
+      <c r="IK22" s="4"/>
+      <c r="IL22" s="4"/>
+      <c r="IM22" s="4"/>
+      <c r="IN22" s="4"/>
+      <c r="IO22" s="4"/>
+      <c r="IP22" s="4"/>
+      <c r="IQ22" s="4"/>
+      <c r="IR22" s="4"/>
+      <c r="IS22" s="4"/>
+      <c r="IT22" s="4"/>
     </row>
-    <row r="29" spans="1:256">
-      <c r="A29" s="6" t="inlineStr">
+    <row r="25" spans="1:256">
+      <c r="A25" s="5" t="inlineStr">
         <is>
           <t>babu1993.py</t>
         </is>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
-      <c r="Y29" s="6"/>
-      <c r="Z29" s="6"/>
-      <c r="AA29" s="6"/>
-      <c r="AB29" s="6"/>
-      <c r="AC29" s="6"/>
-      <c r="AD29" s="6"/>
-      <c r="AE29" s="6"/>
-      <c r="AF29" s="6"/>
-      <c r="AG29" s="6"/>
-      <c r="AH29" s="6"/>
-      <c r="AI29" s="6"/>
-      <c r="AJ29" s="6"/>
-      <c r="AK29" s="6"/>
-      <c r="AL29" s="6"/>
-      <c r="AM29" s="6"/>
-      <c r="AN29" s="6"/>
-      <c r="AO29" s="6"/>
-      <c r="AP29" s="6"/>
-      <c r="AQ29" s="6"/>
-      <c r="AR29" s="6"/>
-      <c r="AS29" s="6"/>
-      <c r="AT29" s="6"/>
-      <c r="AU29" s="6"/>
-      <c r="AV29" s="6"/>
-      <c r="AW29" s="6"/>
-      <c r="AX29" s="6"/>
-      <c r="AY29" s="6"/>
-      <c r="AZ29" s="6"/>
-      <c r="BA29" s="6"/>
-      <c r="BB29" s="6"/>
-      <c r="BC29" s="6"/>
-      <c r="BD29" s="6"/>
-      <c r="BE29" s="6"/>
-      <c r="BF29" s="6"/>
-      <c r="BG29" s="6"/>
-      <c r="BH29" s="6"/>
-      <c r="BI29" s="6"/>
-      <c r="BJ29" s="6"/>
-      <c r="BK29" s="6"/>
-      <c r="BL29" s="6"/>
-      <c r="BM29" s="6"/>
-      <c r="BN29" s="6"/>
-      <c r="BO29" s="6"/>
-      <c r="BP29" s="6"/>
-      <c r="BQ29" s="6"/>
-      <c r="BR29" s="6"/>
-      <c r="BS29" s="6"/>
-      <c r="BT29" s="6"/>
-      <c r="BU29" s="6"/>
-      <c r="BV29" s="6"/>
-      <c r="BW29" s="6"/>
-      <c r="BX29" s="6"/>
-      <c r="BY29" s="6"/>
-      <c r="BZ29" s="6"/>
-      <c r="CA29" s="6"/>
-      <c r="CB29" s="6"/>
-      <c r="CC29" s="6"/>
-      <c r="CD29" s="6"/>
-      <c r="CE29" s="6"/>
-      <c r="CF29" s="6"/>
-      <c r="CG29" s="6"/>
-      <c r="CH29" s="6"/>
-      <c r="CI29" s="6"/>
-      <c r="CJ29" s="6"/>
-      <c r="CK29" s="6"/>
-      <c r="CL29" s="6"/>
-      <c r="CM29" s="6"/>
-      <c r="CN29" s="6"/>
-      <c r="CO29" s="6"/>
-      <c r="CP29" s="6"/>
-      <c r="CQ29" s="6"/>
-      <c r="CR29" s="6"/>
-      <c r="CS29" s="6"/>
-      <c r="CT29" s="6"/>
-      <c r="CU29" s="6"/>
-      <c r="CV29" s="6"/>
-      <c r="CW29" s="6"/>
-      <c r="CX29" s="6"/>
-      <c r="CY29" s="6"/>
-      <c r="CZ29" s="6"/>
-      <c r="DA29" s="6"/>
-      <c r="DB29" s="6"/>
-      <c r="DC29" s="6"/>
-      <c r="DD29" s="6"/>
-      <c r="DE29" s="6"/>
-      <c r="DF29" s="6"/>
-      <c r="DG29" s="6"/>
-      <c r="DH29" s="6"/>
-      <c r="DI29" s="6"/>
-      <c r="DJ29" s="6"/>
-      <c r="DK29" s="6"/>
-      <c r="DL29" s="6"/>
-      <c r="DM29" s="6"/>
-      <c r="DN29" s="6"/>
-      <c r="DO29" s="6"/>
-      <c r="DP29" s="6"/>
-      <c r="DQ29" s="6"/>
-      <c r="DR29" s="6"/>
-      <c r="DS29" s="6"/>
-      <c r="DT29" s="6"/>
-      <c r="DU29" s="6"/>
-      <c r="DV29" s="6"/>
-      <c r="DW29" s="6"/>
-      <c r="DX29" s="6"/>
-      <c r="DY29" s="6"/>
-      <c r="DZ29" s="6"/>
-      <c r="EA29" s="6"/>
-      <c r="EB29" s="6"/>
-      <c r="EC29" s="6"/>
-      <c r="ED29" s="6"/>
-      <c r="EE29" s="6"/>
-      <c r="EF29" s="6"/>
-      <c r="EG29" s="6"/>
-      <c r="EH29" s="6"/>
-      <c r="EI29" s="6"/>
-      <c r="EJ29" s="6"/>
-      <c r="EK29" s="6"/>
-      <c r="EL29" s="6"/>
-      <c r="EM29" s="6"/>
-      <c r="EN29" s="6"/>
-      <c r="EO29" s="6"/>
-      <c r="EP29" s="6"/>
-      <c r="EQ29" s="6"/>
-      <c r="ER29" s="6"/>
-      <c r="ES29" s="6"/>
-      <c r="ET29" s="6"/>
-      <c r="EU29" s="6"/>
-      <c r="EV29" s="6"/>
-      <c r="EW29" s="6"/>
-      <c r="EX29" s="6"/>
-      <c r="EY29" s="6"/>
-      <c r="EZ29" s="6"/>
-      <c r="FA29" s="6"/>
-      <c r="FB29" s="6"/>
-      <c r="FC29" s="6"/>
-      <c r="FD29" s="6"/>
-      <c r="FE29" s="6"/>
-      <c r="FF29" s="6"/>
-      <c r="FG29" s="6"/>
-      <c r="FH29" s="6"/>
-      <c r="FI29" s="6"/>
-      <c r="FJ29" s="6"/>
-      <c r="FK29" s="6"/>
-      <c r="FL29" s="6"/>
-      <c r="FM29" s="6"/>
-      <c r="FN29" s="6"/>
-      <c r="FO29" s="6"/>
-      <c r="FP29" s="6"/>
-      <c r="FQ29" s="6"/>
-      <c r="FR29" s="6"/>
-      <c r="FS29" s="6"/>
-      <c r="FT29" s="6"/>
-      <c r="FU29" s="6"/>
-      <c r="FV29" s="6"/>
-      <c r="FW29" s="6"/>
-      <c r="FX29" s="6"/>
-      <c r="FY29" s="6"/>
-      <c r="FZ29" s="6"/>
-      <c r="GA29" s="6"/>
-      <c r="GB29" s="6"/>
-      <c r="GC29" s="6"/>
-      <c r="GD29" s="6"/>
-      <c r="GE29" s="6"/>
-      <c r="GF29" s="6"/>
-      <c r="GG29" s="6"/>
-      <c r="GH29" s="6"/>
-      <c r="GI29" s="6"/>
-      <c r="GJ29" s="6"/>
-      <c r="GK29" s="6"/>
-      <c r="GL29" s="6"/>
-      <c r="GM29" s="6"/>
-      <c r="GN29" s="6"/>
-      <c r="GO29" s="6"/>
-      <c r="GP29" s="6"/>
-      <c r="GQ29" s="6"/>
-      <c r="GR29" s="6"/>
-      <c r="GS29" s="6"/>
-      <c r="GT29" s="6"/>
-      <c r="GU29" s="6"/>
-      <c r="GV29" s="6"/>
-      <c r="GW29" s="6"/>
-      <c r="GX29" s="6"/>
-      <c r="GY29" s="6"/>
-      <c r="GZ29" s="6"/>
-      <c r="HA29" s="6"/>
-      <c r="HB29" s="6"/>
-      <c r="HC29" s="6"/>
-      <c r="HD29" s="6"/>
-      <c r="HE29" s="6"/>
-      <c r="HF29" s="6"/>
-      <c r="HG29" s="6"/>
-      <c r="HH29" s="6"/>
-      <c r="HI29" s="6"/>
-      <c r="HJ29" s="6"/>
-      <c r="HK29" s="6"/>
-      <c r="HL29" s="6"/>
-      <c r="HM29" s="6"/>
-      <c r="HN29" s="6"/>
-      <c r="HO29" s="6"/>
-      <c r="HP29" s="6"/>
-      <c r="HQ29" s="6"/>
-      <c r="HR29" s="6"/>
-      <c r="HS29" s="6"/>
-      <c r="HT29" s="6"/>
-      <c r="HU29" s="6"/>
-      <c r="HV29" s="6"/>
-      <c r="HW29" s="6"/>
-      <c r="HX29" s="6"/>
-      <c r="HY29" s="6"/>
-      <c r="HZ29" s="6"/>
-      <c r="IA29" s="6"/>
-      <c r="IB29" s="6"/>
-      <c r="IC29" s="6"/>
-      <c r="ID29" s="6"/>
-      <c r="IE29" s="6"/>
-      <c r="IF29" s="6"/>
-      <c r="IG29" s="6"/>
-      <c r="IH29" s="6"/>
-      <c r="II29" s="6"/>
-      <c r="IJ29" s="6"/>
-      <c r="IK29" s="6"/>
-      <c r="IL29" s="6"/>
-      <c r="IM29" s="6"/>
-      <c r="IN29" s="6"/>
-      <c r="IO29" s="6"/>
-      <c r="IP29" s="6"/>
-      <c r="IQ29" s="6"/>
-      <c r="IR29" s="6"/>
-      <c r="IS29" s="6"/>
-      <c r="IT29" s="6"/>
+      <c r="B25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+      <c r="AF25" s="5"/>
+      <c r="AG25" s="5"/>
+      <c r="AH25" s="5"/>
+      <c r="AI25" s="5"/>
+      <c r="AJ25" s="5"/>
+      <c r="AK25" s="5"/>
+      <c r="AL25" s="5"/>
+      <c r="AM25" s="5"/>
+      <c r="AN25" s="5"/>
+      <c r="AO25" s="5"/>
+      <c r="AP25" s="5"/>
+      <c r="AQ25" s="5"/>
+      <c r="AR25" s="5"/>
+      <c r="AS25" s="5"/>
+      <c r="AT25" s="5"/>
+      <c r="AU25" s="5"/>
+      <c r="AV25" s="5"/>
+      <c r="AW25" s="5"/>
+      <c r="AX25" s="5"/>
+      <c r="AY25" s="5"/>
+      <c r="AZ25" s="5"/>
+      <c r="BA25" s="5"/>
+      <c r="BB25" s="5"/>
+      <c r="BC25" s="5"/>
+      <c r="BD25" s="5"/>
+      <c r="BE25" s="5"/>
+      <c r="BF25" s="5"/>
+      <c r="BG25" s="5"/>
+      <c r="BH25" s="5"/>
+      <c r="BI25" s="5"/>
+      <c r="BJ25" s="5"/>
+      <c r="BK25" s="5"/>
+      <c r="BL25" s="5"/>
+      <c r="BM25" s="5"/>
+      <c r="BN25" s="5"/>
+      <c r="BO25" s="5"/>
+      <c r="BP25" s="5"/>
+      <c r="BQ25" s="5"/>
+      <c r="BR25" s="5"/>
+      <c r="BS25" s="5"/>
+      <c r="BT25" s="5"/>
+      <c r="BU25" s="5"/>
+      <c r="BV25" s="5"/>
+      <c r="BW25" s="5"/>
+      <c r="BX25" s="5"/>
+      <c r="BY25" s="5"/>
+      <c r="BZ25" s="5"/>
+      <c r="CA25" s="5"/>
+      <c r="CB25" s="5"/>
+      <c r="CC25" s="5"/>
+      <c r="CD25" s="5"/>
+      <c r="CE25" s="5"/>
+      <c r="CF25" s="5"/>
+      <c r="CG25" s="5"/>
+      <c r="CH25" s="5"/>
+      <c r="CI25" s="5"/>
+      <c r="CJ25" s="5"/>
+      <c r="CK25" s="5"/>
+      <c r="CL25" s="5"/>
+      <c r="CM25" s="5"/>
+      <c r="CN25" s="5"/>
+      <c r="CO25" s="5"/>
+      <c r="CP25" s="5"/>
+      <c r="CQ25" s="5"/>
+      <c r="CR25" s="5"/>
+      <c r="CS25" s="5"/>
+      <c r="CT25" s="5"/>
+      <c r="CU25" s="5"/>
+      <c r="CV25" s="5"/>
+      <c r="CW25" s="5"/>
+      <c r="CX25" s="5"/>
+      <c r="CY25" s="5"/>
+      <c r="CZ25" s="5"/>
+      <c r="DA25" s="5"/>
+      <c r="DB25" s="5"/>
+      <c r="DC25" s="5"/>
+      <c r="DD25" s="5"/>
+      <c r="DE25" s="5"/>
+      <c r="DF25" s="5"/>
+      <c r="DG25" s="5"/>
+      <c r="DH25" s="5"/>
+      <c r="DI25" s="5"/>
+      <c r="DJ25" s="5"/>
+      <c r="DK25" s="5"/>
+      <c r="DL25" s="5"/>
+      <c r="DM25" s="5"/>
+      <c r="DN25" s="5"/>
+      <c r="DO25" s="5"/>
+      <c r="DP25" s="5"/>
+      <c r="DQ25" s="5"/>
+      <c r="DR25" s="5"/>
+      <c r="DS25" s="5"/>
+      <c r="DT25" s="5"/>
+      <c r="DU25" s="5"/>
+      <c r="DV25" s="5"/>
+      <c r="DW25" s="5"/>
+      <c r="DX25" s="5"/>
+      <c r="DY25" s="5"/>
+      <c r="DZ25" s="5"/>
+      <c r="EA25" s="5"/>
+      <c r="EB25" s="5"/>
+      <c r="EC25" s="5"/>
+      <c r="ED25" s="5"/>
+      <c r="EE25" s="5"/>
+      <c r="EF25" s="5"/>
+      <c r="EG25" s="5"/>
+      <c r="EH25" s="5"/>
+      <c r="EI25" s="5"/>
+      <c r="EJ25" s="5"/>
+      <c r="EK25" s="5"/>
+      <c r="EL25" s="5"/>
+      <c r="EM25" s="5"/>
+      <c r="EN25" s="5"/>
+      <c r="EO25" s="5"/>
+      <c r="EP25" s="5"/>
+      <c r="EQ25" s="5"/>
+      <c r="ER25" s="5"/>
+      <c r="ES25" s="5"/>
+      <c r="ET25" s="5"/>
+      <c r="EU25" s="5"/>
+      <c r="EV25" s="5"/>
+      <c r="EW25" s="5"/>
+      <c r="EX25" s="5"/>
+      <c r="EY25" s="5"/>
+      <c r="EZ25" s="5"/>
+      <c r="FA25" s="5"/>
+      <c r="FB25" s="5"/>
+      <c r="FC25" s="5"/>
+      <c r="FD25" s="5"/>
+      <c r="FE25" s="5"/>
+      <c r="FF25" s="5"/>
+      <c r="FG25" s="5"/>
+      <c r="FH25" s="5"/>
+      <c r="FI25" s="5"/>
+      <c r="FJ25" s="5"/>
+      <c r="FK25" s="5"/>
+      <c r="FL25" s="5"/>
+      <c r="FM25" s="5"/>
+      <c r="FN25" s="5"/>
+      <c r="FO25" s="5"/>
+      <c r="FP25" s="5"/>
+      <c r="FQ25" s="5"/>
+      <c r="FR25" s="5"/>
+      <c r="FS25" s="5"/>
+      <c r="FT25" s="5"/>
+      <c r="FU25" s="5"/>
+      <c r="FV25" s="5"/>
+      <c r="FW25" s="5"/>
+      <c r="FX25" s="5"/>
+      <c r="FY25" s="5"/>
+      <c r="FZ25" s="5"/>
+      <c r="GA25" s="5"/>
+      <c r="GB25" s="5"/>
+      <c r="GC25" s="5"/>
+      <c r="GD25" s="5"/>
+      <c r="GE25" s="5"/>
+      <c r="GF25" s="5"/>
+      <c r="GG25" s="5"/>
+      <c r="GH25" s="5"/>
+      <c r="GI25" s="5"/>
+      <c r="GJ25" s="5"/>
+      <c r="GK25" s="5"/>
+      <c r="GL25" s="5"/>
+      <c r="GM25" s="5"/>
+      <c r="GN25" s="5"/>
+      <c r="GO25" s="5"/>
+      <c r="GP25" s="5"/>
+      <c r="GQ25" s="5"/>
+      <c r="GR25" s="5"/>
+      <c r="GS25" s="5"/>
+      <c r="GT25" s="5"/>
+      <c r="GU25" s="5"/>
+      <c r="GV25" s="5"/>
+      <c r="GW25" s="5"/>
+      <c r="GX25" s="5"/>
+      <c r="GY25" s="5"/>
+      <c r="GZ25" s="5"/>
+      <c r="HA25" s="5"/>
+      <c r="HB25" s="5"/>
+      <c r="HC25" s="5"/>
+      <c r="HD25" s="5"/>
+      <c r="HE25" s="5"/>
+      <c r="HF25" s="5"/>
+      <c r="HG25" s="5"/>
+      <c r="HH25" s="5"/>
+      <c r="HI25" s="5"/>
+      <c r="HJ25" s="5"/>
+      <c r="HK25" s="5"/>
+      <c r="HL25" s="5"/>
+      <c r="HM25" s="5"/>
+      <c r="HN25" s="5"/>
+      <c r="HO25" s="5"/>
+      <c r="HP25" s="5"/>
+      <c r="HQ25" s="5"/>
+      <c r="HR25" s="5"/>
+      <c r="HS25" s="5"/>
+      <c r="HT25" s="5"/>
+      <c r="HU25" s="5"/>
+      <c r="HV25" s="5"/>
+      <c r="HW25" s="5"/>
+      <c r="HX25" s="5"/>
+      <c r="HY25" s="5"/>
+      <c r="HZ25" s="5"/>
+      <c r="IA25" s="5"/>
+      <c r="IB25" s="5"/>
+      <c r="IC25" s="5"/>
+      <c r="ID25" s="5"/>
+      <c r="IE25" s="5"/>
+      <c r="IF25" s="5"/>
+      <c r="IG25" s="5"/>
+      <c r="IH25" s="5"/>
+      <c r="II25" s="5"/>
+      <c r="IJ25" s="5"/>
+      <c r="IK25" s="5"/>
+      <c r="IL25" s="5"/>
+      <c r="IM25" s="5"/>
+      <c r="IN25" s="5"/>
+      <c r="IO25" s="5"/>
+      <c r="IP25" s="5"/>
+      <c r="IQ25" s="5"/>
+      <c r="IR25" s="5"/>
+      <c r="IS25" s="5"/>
+      <c r="IT25" s="5"/>
+    </row>
+    <row r="65533" spans="1:256">
+      <c r="A65533" s="0"/>
+      <c r="B65533" s="0"/>
+      <c r="C65533" s="0"/>
+      <c r="D65533" s="0"/>
+      <c r="E65533" s="0"/>
+      <c r="F65533" s="0"/>
+      <c r="G65533" s="0"/>
+      <c r="H65533" s="0"/>
+      <c r="I65533" s="0"/>
+      <c r="J65533" s="0"/>
+      <c r="K65533" s="0"/>
+      <c r="L65533" s="0"/>
+      <c r="M65533" s="0"/>
+      <c r="N65533" s="0"/>
+      <c r="O65533" s="0"/>
+      <c r="P65533" s="0"/>
+      <c r="Q65533" s="0"/>
+      <c r="R65533" s="0"/>
+      <c r="S65533" s="0"/>
+      <c r="T65533" s="0"/>
+      <c r="U65533" s="0"/>
+      <c r="V65533" s="0"/>
+      <c r="W65533" s="0"/>
+      <c r="X65533" s="0"/>
+      <c r="Y65533" s="0"/>
+      <c r="Z65533" s="0"/>
+      <c r="AA65533" s="0"/>
+      <c r="AB65533" s="0"/>
+      <c r="AC65533" s="0"/>
+      <c r="AD65533" s="0"/>
+      <c r="AE65533" s="0"/>
+      <c r="AF65533" s="0"/>
+      <c r="AG65533" s="0"/>
+      <c r="AH65533" s="0"/>
+      <c r="AI65533" s="0"/>
+      <c r="AJ65533" s="0"/>
+      <c r="AK65533" s="0"/>
+      <c r="AL65533" s="0"/>
+      <c r="AM65533" s="0"/>
+      <c r="AN65533" s="0"/>
+      <c r="AO65533" s="0"/>
+      <c r="AP65533" s="0"/>
+      <c r="AQ65533" s="0"/>
+      <c r="AR65533" s="0"/>
+      <c r="AS65533" s="0"/>
+      <c r="AT65533" s="0"/>
+      <c r="AU65533" s="0"/>
+      <c r="AV65533" s="0"/>
+      <c r="AW65533" s="0"/>
+      <c r="AX65533" s="0"/>
+      <c r="AY65533" s="0"/>
+      <c r="AZ65533" s="0"/>
+      <c r="BA65533" s="0"/>
+      <c r="BB65533" s="0"/>
+      <c r="BC65533" s="0"/>
+      <c r="BD65533" s="0"/>
+      <c r="BE65533" s="0"/>
+      <c r="BF65533" s="0"/>
+      <c r="BG65533" s="0"/>
+      <c r="BH65533" s="0"/>
+      <c r="BI65533" s="0"/>
+      <c r="BJ65533" s="0"/>
+      <c r="BK65533" s="0"/>
+      <c r="BL65533" s="0"/>
+      <c r="BM65533" s="0"/>
+      <c r="BN65533" s="0"/>
+      <c r="BO65533" s="0"/>
+      <c r="BP65533" s="0"/>
+      <c r="BQ65533" s="0"/>
+      <c r="BR65533" s="0"/>
+      <c r="BS65533" s="0"/>
+      <c r="BT65533" s="0"/>
+      <c r="BU65533" s="0"/>
+      <c r="BV65533" s="0"/>
+      <c r="BW65533" s="0"/>
+      <c r="BX65533" s="0"/>
+      <c r="BY65533" s="0"/>
+      <c r="BZ65533" s="0"/>
+      <c r="CA65533" s="0"/>
+      <c r="CB65533" s="0"/>
+      <c r="CC65533" s="0"/>
+      <c r="CD65533" s="0"/>
+      <c r="CE65533" s="0"/>
+      <c r="CF65533" s="0"/>
+      <c r="CG65533" s="0"/>
+      <c r="CH65533" s="0"/>
+      <c r="CI65533" s="0"/>
+      <c r="CJ65533" s="0"/>
+      <c r="CK65533" s="0"/>
+      <c r="CL65533" s="0"/>
+      <c r="CM65533" s="0"/>
+      <c r="CN65533" s="0"/>
+      <c r="CO65533" s="0"/>
+      <c r="CP65533" s="0"/>
+      <c r="CQ65533" s="0"/>
+      <c r="CR65533" s="0"/>
+      <c r="CS65533" s="0"/>
+      <c r="CT65533" s="0"/>
+      <c r="CU65533" s="0"/>
+      <c r="CV65533" s="0"/>
+      <c r="CW65533" s="0"/>
+      <c r="CX65533" s="0"/>
+      <c r="CY65533" s="0"/>
+      <c r="CZ65533" s="0"/>
+      <c r="DA65533" s="0"/>
+      <c r="DB65533" s="0"/>
+      <c r="DC65533" s="0"/>
+      <c r="DD65533" s="0"/>
+      <c r="DE65533" s="0"/>
+      <c r="DF65533" s="0"/>
+      <c r="DG65533" s="0"/>
+      <c r="DH65533" s="0"/>
+      <c r="DI65533" s="0"/>
+      <c r="DJ65533" s="0"/>
+      <c r="DK65533" s="0"/>
+      <c r="DL65533" s="0"/>
+      <c r="DM65533" s="0"/>
+      <c r="DN65533" s="0"/>
+      <c r="DO65533" s="0"/>
+      <c r="DP65533" s="0"/>
+      <c r="DQ65533" s="0"/>
+      <c r="DR65533" s="0"/>
+      <c r="DS65533" s="0"/>
+      <c r="DT65533" s="0"/>
+      <c r="DU65533" s="0"/>
+      <c r="DV65533" s="0"/>
+      <c r="DW65533" s="0"/>
+      <c r="DX65533" s="0"/>
+      <c r="DY65533" s="0"/>
+      <c r="DZ65533" s="0"/>
+      <c r="EA65533" s="0"/>
+      <c r="EB65533" s="0"/>
+      <c r="EC65533" s="0"/>
+      <c r="ED65533" s="0"/>
+      <c r="EE65533" s="0"/>
+      <c r="EF65533" s="0"/>
+      <c r="EG65533" s="0"/>
+      <c r="EH65533" s="0"/>
+      <c r="EI65533" s="0"/>
+      <c r="EJ65533" s="0"/>
+      <c r="EK65533" s="0"/>
+      <c r="EL65533" s="0"/>
+      <c r="EM65533" s="0"/>
+      <c r="EN65533" s="0"/>
+      <c r="EO65533" s="0"/>
+      <c r="EP65533" s="0"/>
+      <c r="EQ65533" s="0"/>
+      <c r="ER65533" s="0"/>
+      <c r="ES65533" s="0"/>
+      <c r="ET65533" s="0"/>
+      <c r="EU65533" s="0"/>
+      <c r="EV65533" s="0"/>
+      <c r="EW65533" s="0"/>
+      <c r="EX65533" s="0"/>
+      <c r="EY65533" s="0"/>
+      <c r="EZ65533" s="0"/>
+      <c r="FA65533" s="0"/>
+      <c r="FB65533" s="0"/>
+      <c r="FC65533" s="0"/>
+      <c r="FD65533" s="0"/>
+      <c r="FE65533" s="0"/>
+      <c r="FF65533" s="0"/>
+      <c r="FG65533" s="0"/>
+      <c r="FH65533" s="0"/>
+      <c r="FI65533" s="0"/>
+      <c r="FJ65533" s="0"/>
+      <c r="FK65533" s="0"/>
+      <c r="FL65533" s="0"/>
+      <c r="FM65533" s="0"/>
+      <c r="FN65533" s="0"/>
+      <c r="FO65533" s="0"/>
+      <c r="FP65533" s="0"/>
+      <c r="FQ65533" s="0"/>
+      <c r="FR65533" s="0"/>
+      <c r="FS65533" s="0"/>
+      <c r="FT65533" s="0"/>
+      <c r="FU65533" s="0"/>
+      <c r="FV65533" s="0"/>
+      <c r="FW65533" s="0"/>
+      <c r="FX65533" s="0"/>
+      <c r="FY65533" s="0"/>
+      <c r="FZ65533" s="0"/>
+      <c r="GA65533" s="0"/>
+      <c r="GB65533" s="0"/>
+      <c r="GC65533" s="0"/>
+      <c r="GD65533" s="0"/>
+      <c r="GE65533" s="0"/>
+      <c r="GF65533" s="0"/>
+      <c r="GG65533" s="0"/>
+      <c r="GH65533" s="0"/>
+      <c r="GI65533" s="0"/>
+      <c r="GJ65533" s="0"/>
+      <c r="GK65533" s="0"/>
+      <c r="GL65533" s="0"/>
+      <c r="GM65533" s="0"/>
+      <c r="GN65533" s="0"/>
+      <c r="GO65533" s="0"/>
+      <c r="GP65533" s="0"/>
+      <c r="GQ65533" s="0"/>
+      <c r="GR65533" s="0"/>
+      <c r="GS65533" s="0"/>
+      <c r="GT65533" s="0"/>
+      <c r="GU65533" s="0"/>
+      <c r="GV65533" s="0"/>
+      <c r="GW65533" s="0"/>
+      <c r="GX65533" s="0"/>
+      <c r="GY65533" s="0"/>
+      <c r="GZ65533" s="0"/>
+      <c r="HA65533" s="0"/>
+      <c r="HB65533" s="0"/>
+      <c r="HC65533" s="0"/>
+      <c r="HD65533" s="0"/>
+      <c r="HE65533" s="0"/>
+      <c r="HF65533" s="0"/>
+      <c r="HG65533" s="0"/>
+      <c r="HH65533" s="0"/>
+      <c r="HI65533" s="0"/>
+      <c r="HJ65533" s="0"/>
+      <c r="HK65533" s="0"/>
+      <c r="HL65533" s="0"/>
+      <c r="HM65533" s="0"/>
+      <c r="HN65533" s="0"/>
+      <c r="HO65533" s="0"/>
+      <c r="HP65533" s="0"/>
+      <c r="HQ65533" s="0"/>
+      <c r="HR65533" s="0"/>
+      <c r="HS65533" s="0"/>
+      <c r="HT65533" s="0"/>
+      <c r="HU65533" s="0"/>
+      <c r="HV65533" s="0"/>
+      <c r="HW65533" s="0"/>
+      <c r="HX65533" s="0"/>
+      <c r="HY65533" s="0"/>
+      <c r="HZ65533" s="0"/>
+      <c r="IA65533" s="0"/>
+      <c r="IB65533" s="0"/>
+      <c r="IC65533" s="0"/>
+      <c r="ID65533" s="0"/>
+      <c r="IE65533" s="0"/>
+      <c r="IF65533" s="0"/>
+      <c r="IG65533" s="0"/>
+      <c r="IH65533" s="0"/>
+      <c r="II65533" s="0"/>
+      <c r="IJ65533" s="0"/>
+      <c r="IK65533" s="0"/>
+      <c r="IL65533" s="0"/>
+      <c r="IM65533" s="0"/>
+      <c r="IN65533" s="0"/>
+      <c r="IO65533" s="0"/>
+      <c r="IP65533" s="0"/>
+      <c r="IQ65533" s="0"/>
+      <c r="IR65533" s="0"/>
+      <c r="IS65533" s="0"/>
+      <c r="IT65533" s="0"/>
+      <c r="IU65533" s="0"/>
+      <c r="IV65533" s="0"/>
+    </row>
+    <row r="65534" spans="1:256">
+      <c r="A65534" s="0"/>
+      <c r="B65534" s="0"/>
+      <c r="C65534" s="0"/>
+      <c r="D65534" s="0"/>
+      <c r="E65534" s="0"/>
+      <c r="F65534" s="0"/>
+      <c r="G65534" s="0"/>
+      <c r="H65534" s="0"/>
+      <c r="I65534" s="0"/>
+      <c r="J65534" s="0"/>
+      <c r="K65534" s="0"/>
+      <c r="L65534" s="0"/>
+      <c r="M65534" s="0"/>
+      <c r="N65534" s="0"/>
+      <c r="O65534" s="0"/>
+      <c r="P65534" s="0"/>
+      <c r="Q65534" s="0"/>
+      <c r="R65534" s="0"/>
+      <c r="S65534" s="0"/>
+      <c r="T65534" s="0"/>
+      <c r="U65534" s="0"/>
+      <c r="V65534" s="0"/>
+      <c r="W65534" s="0"/>
+      <c r="X65534" s="0"/>
+      <c r="Y65534" s="0"/>
+      <c r="Z65534" s="0"/>
+      <c r="AA65534" s="0"/>
+      <c r="AB65534" s="0"/>
+      <c r="AC65534" s="0"/>
+      <c r="AD65534" s="0"/>
+      <c r="AE65534" s="0"/>
+      <c r="AF65534" s="0"/>
+      <c r="AG65534" s="0"/>
+      <c r="AH65534" s="0"/>
+      <c r="AI65534" s="0"/>
+      <c r="AJ65534" s="0"/>
+      <c r="AK65534" s="0"/>
+      <c r="AL65534" s="0"/>
+      <c r="AM65534" s="0"/>
+      <c r="AN65534" s="0"/>
+      <c r="AO65534" s="0"/>
+      <c r="AP65534" s="0"/>
+      <c r="AQ65534" s="0"/>
+      <c r="AR65534" s="0"/>
+      <c r="AS65534" s="0"/>
+      <c r="AT65534" s="0"/>
+      <c r="AU65534" s="0"/>
+      <c r="AV65534" s="0"/>
+      <c r="AW65534" s="0"/>
+      <c r="AX65534" s="0"/>
+      <c r="AY65534" s="0"/>
+      <c r="AZ65534" s="0"/>
+      <c r="BA65534" s="0"/>
+      <c r="BB65534" s="0"/>
+      <c r="BC65534" s="0"/>
+      <c r="BD65534" s="0"/>
+      <c r="BE65534" s="0"/>
+      <c r="BF65534" s="0"/>
+      <c r="BG65534" s="0"/>
+      <c r="BH65534" s="0"/>
+      <c r="BI65534" s="0"/>
+      <c r="BJ65534" s="0"/>
+      <c r="BK65534" s="0"/>
+      <c r="BL65534" s="0"/>
+      <c r="BM65534" s="0"/>
+      <c r="BN65534" s="0"/>
+      <c r="BO65534" s="0"/>
+      <c r="BP65534" s="0"/>
+      <c r="BQ65534" s="0"/>
+      <c r="BR65534" s="0"/>
+      <c r="BS65534" s="0"/>
+      <c r="BT65534" s="0"/>
+      <c r="BU65534" s="0"/>
+      <c r="BV65534" s="0"/>
+      <c r="BW65534" s="0"/>
+      <c r="BX65534" s="0"/>
+      <c r="BY65534" s="0"/>
+      <c r="BZ65534" s="0"/>
+      <c r="CA65534" s="0"/>
+      <c r="CB65534" s="0"/>
+      <c r="CC65534" s="0"/>
+      <c r="CD65534" s="0"/>
+      <c r="CE65534" s="0"/>
+      <c r="CF65534" s="0"/>
+      <c r="CG65534" s="0"/>
+      <c r="CH65534" s="0"/>
+      <c r="CI65534" s="0"/>
+      <c r="CJ65534" s="0"/>
+      <c r="CK65534" s="0"/>
+      <c r="CL65534" s="0"/>
+      <c r="CM65534" s="0"/>
+      <c r="CN65534" s="0"/>
+      <c r="CO65534" s="0"/>
+      <c r="CP65534" s="0"/>
+      <c r="CQ65534" s="0"/>
+      <c r="CR65534" s="0"/>
+      <c r="CS65534" s="0"/>
+      <c r="CT65534" s="0"/>
+      <c r="CU65534" s="0"/>
+      <c r="CV65534" s="0"/>
+      <c r="CW65534" s="0"/>
+      <c r="CX65534" s="0"/>
+      <c r="CY65534" s="0"/>
+      <c r="CZ65534" s="0"/>
+      <c r="DA65534" s="0"/>
+      <c r="DB65534" s="0"/>
+      <c r="DC65534" s="0"/>
+      <c r="DD65534" s="0"/>
+      <c r="DE65534" s="0"/>
+      <c r="DF65534" s="0"/>
+      <c r="DG65534" s="0"/>
+      <c r="DH65534" s="0"/>
+      <c r="DI65534" s="0"/>
+      <c r="DJ65534" s="0"/>
+      <c r="DK65534" s="0"/>
+      <c r="DL65534" s="0"/>
+      <c r="DM65534" s="0"/>
+      <c r="DN65534" s="0"/>
+      <c r="DO65534" s="0"/>
+      <c r="DP65534" s="0"/>
+      <c r="DQ65534" s="0"/>
+      <c r="DR65534" s="0"/>
+      <c r="DS65534" s="0"/>
+      <c r="DT65534" s="0"/>
+      <c r="DU65534" s="0"/>
+      <c r="DV65534" s="0"/>
+      <c r="DW65534" s="0"/>
+      <c r="DX65534" s="0"/>
+      <c r="DY65534" s="0"/>
+      <c r="DZ65534" s="0"/>
+      <c r="EA65534" s="0"/>
+      <c r="EB65534" s="0"/>
+      <c r="EC65534" s="0"/>
+      <c r="ED65534" s="0"/>
+      <c r="EE65534" s="0"/>
+      <c r="EF65534" s="0"/>
+      <c r="EG65534" s="0"/>
+      <c r="EH65534" s="0"/>
+      <c r="EI65534" s="0"/>
+      <c r="EJ65534" s="0"/>
+      <c r="EK65534" s="0"/>
+      <c r="EL65534" s="0"/>
+      <c r="EM65534" s="0"/>
+      <c r="EN65534" s="0"/>
+      <c r="EO65534" s="0"/>
+      <c r="EP65534" s="0"/>
+      <c r="EQ65534" s="0"/>
+      <c r="ER65534" s="0"/>
+      <c r="ES65534" s="0"/>
+      <c r="ET65534" s="0"/>
+      <c r="EU65534" s="0"/>
+      <c r="EV65534" s="0"/>
+      <c r="EW65534" s="0"/>
+      <c r="EX65534" s="0"/>
+      <c r="EY65534" s="0"/>
+      <c r="EZ65534" s="0"/>
+      <c r="FA65534" s="0"/>
+      <c r="FB65534" s="0"/>
+      <c r="FC65534" s="0"/>
+      <c r="FD65534" s="0"/>
+      <c r="FE65534" s="0"/>
+      <c r="FF65534" s="0"/>
+      <c r="FG65534" s="0"/>
+      <c r="FH65534" s="0"/>
+      <c r="FI65534" s="0"/>
+      <c r="FJ65534" s="0"/>
+      <c r="FK65534" s="0"/>
+      <c r="FL65534" s="0"/>
+      <c r="FM65534" s="0"/>
+      <c r="FN65534" s="0"/>
+      <c r="FO65534" s="0"/>
+      <c r="FP65534" s="0"/>
+      <c r="FQ65534" s="0"/>
+      <c r="FR65534" s="0"/>
+      <c r="FS65534" s="0"/>
+      <c r="FT65534" s="0"/>
+      <c r="FU65534" s="0"/>
+      <c r="FV65534" s="0"/>
+      <c r="FW65534" s="0"/>
+      <c r="FX65534" s="0"/>
+      <c r="FY65534" s="0"/>
+      <c r="FZ65534" s="0"/>
+      <c r="GA65534" s="0"/>
+      <c r="GB65534" s="0"/>
+      <c r="GC65534" s="0"/>
+      <c r="GD65534" s="0"/>
+      <c r="GE65534" s="0"/>
+      <c r="GF65534" s="0"/>
+      <c r="GG65534" s="0"/>
+      <c r="GH65534" s="0"/>
+      <c r="GI65534" s="0"/>
+      <c r="GJ65534" s="0"/>
+      <c r="GK65534" s="0"/>
+      <c r="GL65534" s="0"/>
+      <c r="GM65534" s="0"/>
+      <c r="GN65534" s="0"/>
+      <c r="GO65534" s="0"/>
+      <c r="GP65534" s="0"/>
+      <c r="GQ65534" s="0"/>
+      <c r="GR65534" s="0"/>
+      <c r="GS65534" s="0"/>
+      <c r="GT65534" s="0"/>
+      <c r="GU65534" s="0"/>
+      <c r="GV65534" s="0"/>
+      <c r="GW65534" s="0"/>
+      <c r="GX65534" s="0"/>
+      <c r="GY65534" s="0"/>
+      <c r="GZ65534" s="0"/>
+      <c r="HA65534" s="0"/>
+      <c r="HB65534" s="0"/>
+      <c r="HC65534" s="0"/>
+      <c r="HD65534" s="0"/>
+      <c r="HE65534" s="0"/>
+      <c r="HF65534" s="0"/>
+      <c r="HG65534" s="0"/>
+      <c r="HH65534" s="0"/>
+      <c r="HI65534" s="0"/>
+      <c r="HJ65534" s="0"/>
+      <c r="HK65534" s="0"/>
+      <c r="HL65534" s="0"/>
+      <c r="HM65534" s="0"/>
+      <c r="HN65534" s="0"/>
+      <c r="HO65534" s="0"/>
+      <c r="HP65534" s="0"/>
+      <c r="HQ65534" s="0"/>
+      <c r="HR65534" s="0"/>
+      <c r="HS65534" s="0"/>
+      <c r="HT65534" s="0"/>
+      <c r="HU65534" s="0"/>
+      <c r="HV65534" s="0"/>
+      <c r="HW65534" s="0"/>
+      <c r="HX65534" s="0"/>
+      <c r="HY65534" s="0"/>
+      <c r="HZ65534" s="0"/>
+      <c r="IA65534" s="0"/>
+      <c r="IB65534" s="0"/>
+      <c r="IC65534" s="0"/>
+      <c r="ID65534" s="0"/>
+      <c r="IE65534" s="0"/>
+      <c r="IF65534" s="0"/>
+      <c r="IG65534" s="0"/>
+      <c r="IH65534" s="0"/>
+      <c r="II65534" s="0"/>
+      <c r="IJ65534" s="0"/>
+      <c r="IK65534" s="0"/>
+      <c r="IL65534" s="0"/>
+      <c r="IM65534" s="0"/>
+      <c r="IN65534" s="0"/>
+      <c r="IO65534" s="0"/>
+      <c r="IP65534" s="0"/>
+      <c r="IQ65534" s="0"/>
+      <c r="IR65534" s="0"/>
+      <c r="IS65534" s="0"/>
+      <c r="IT65534" s="0"/>
+      <c r="IU65534" s="0"/>
+      <c r="IV65534" s="0"/>
+    </row>
+    <row r="65535" spans="1:256">
+      <c r="A65535" s="0"/>
+      <c r="B65535" s="0"/>
+      <c r="C65535" s="0"/>
+      <c r="D65535" s="0"/>
+      <c r="E65535" s="0"/>
+      <c r="F65535" s="0"/>
+      <c r="G65535" s="0"/>
+      <c r="H65535" s="0"/>
+      <c r="I65535" s="0"/>
+      <c r="J65535" s="0"/>
+      <c r="K65535" s="0"/>
+      <c r="L65535" s="0"/>
+      <c r="M65535" s="0"/>
+      <c r="N65535" s="0"/>
+      <c r="O65535" s="0"/>
+      <c r="P65535" s="0"/>
+      <c r="Q65535" s="0"/>
+      <c r="R65535" s="0"/>
+      <c r="S65535" s="0"/>
+      <c r="T65535" s="0"/>
+      <c r="U65535" s="0"/>
+      <c r="V65535" s="0"/>
+      <c r="W65535" s="0"/>
+      <c r="X65535" s="0"/>
+      <c r="Y65535" s="0"/>
+      <c r="Z65535" s="0"/>
+      <c r="AA65535" s="0"/>
+      <c r="AB65535" s="0"/>
+      <c r="AC65535" s="0"/>
+      <c r="AD65535" s="0"/>
+      <c r="AE65535" s="0"/>
+      <c r="AF65535" s="0"/>
+      <c r="AG65535" s="0"/>
+      <c r="AH65535" s="0"/>
+      <c r="AI65535" s="0"/>
+      <c r="AJ65535" s="0"/>
+      <c r="AK65535" s="0"/>
+      <c r="AL65535" s="0"/>
+      <c r="AM65535" s="0"/>
+      <c r="AN65535" s="0"/>
+      <c r="AO65535" s="0"/>
+      <c r="AP65535" s="0"/>
+      <c r="AQ65535" s="0"/>
+      <c r="AR65535" s="0"/>
+      <c r="AS65535" s="0"/>
+      <c r="AT65535" s="0"/>
+      <c r="AU65535" s="0"/>
+      <c r="AV65535" s="0"/>
+      <c r="AW65535" s="0"/>
+      <c r="AX65535" s="0"/>
+      <c r="AY65535" s="0"/>
+      <c r="AZ65535" s="0"/>
+      <c r="BA65535" s="0"/>
+      <c r="BB65535" s="0"/>
+      <c r="BC65535" s="0"/>
+      <c r="BD65535" s="0"/>
+      <c r="BE65535" s="0"/>
+      <c r="BF65535" s="0"/>
+      <c r="BG65535" s="0"/>
+      <c r="BH65535" s="0"/>
+      <c r="BI65535" s="0"/>
+      <c r="BJ65535" s="0"/>
+      <c r="BK65535" s="0"/>
+      <c r="BL65535" s="0"/>
+      <c r="BM65535" s="0"/>
+      <c r="BN65535" s="0"/>
+      <c r="BO65535" s="0"/>
+      <c r="BP65535" s="0"/>
+      <c r="BQ65535" s="0"/>
+      <c r="BR65535" s="0"/>
+      <c r="BS65535" s="0"/>
+      <c r="BT65535" s="0"/>
+      <c r="BU65535" s="0"/>
+      <c r="BV65535" s="0"/>
+      <c r="BW65535" s="0"/>
+      <c r="BX65535" s="0"/>
+      <c r="BY65535" s="0"/>
+      <c r="BZ65535" s="0"/>
+      <c r="CA65535" s="0"/>
+      <c r="CB65535" s="0"/>
+      <c r="CC65535" s="0"/>
+      <c r="CD65535" s="0"/>
+      <c r="CE65535" s="0"/>
+      <c r="CF65535" s="0"/>
+      <c r="CG65535" s="0"/>
+      <c r="CH65535" s="0"/>
+      <c r="CI65535" s="0"/>
+      <c r="CJ65535" s="0"/>
+      <c r="CK65535" s="0"/>
+      <c r="CL65535" s="0"/>
+      <c r="CM65535" s="0"/>
+      <c r="CN65535" s="0"/>
+      <c r="CO65535" s="0"/>
+      <c r="CP65535" s="0"/>
+      <c r="CQ65535" s="0"/>
+      <c r="CR65535" s="0"/>
+      <c r="CS65535" s="0"/>
+      <c r="CT65535" s="0"/>
+      <c r="CU65535" s="0"/>
+      <c r="CV65535" s="0"/>
+      <c r="CW65535" s="0"/>
+      <c r="CX65535" s="0"/>
+      <c r="CY65535" s="0"/>
+      <c r="CZ65535" s="0"/>
+      <c r="DA65535" s="0"/>
+      <c r="DB65535" s="0"/>
+      <c r="DC65535" s="0"/>
+      <c r="DD65535" s="0"/>
+      <c r="DE65535" s="0"/>
+      <c r="DF65535" s="0"/>
+      <c r="DG65535" s="0"/>
+      <c r="DH65535" s="0"/>
+      <c r="DI65535" s="0"/>
+      <c r="DJ65535" s="0"/>
+      <c r="DK65535" s="0"/>
+      <c r="DL65535" s="0"/>
+      <c r="DM65535" s="0"/>
+      <c r="DN65535" s="0"/>
+      <c r="DO65535" s="0"/>
+      <c r="DP65535" s="0"/>
+      <c r="DQ65535" s="0"/>
+      <c r="DR65535" s="0"/>
+      <c r="DS65535" s="0"/>
+      <c r="DT65535" s="0"/>
+      <c r="DU65535" s="0"/>
+      <c r="DV65535" s="0"/>
+      <c r="DW65535" s="0"/>
+      <c r="DX65535" s="0"/>
+      <c r="DY65535" s="0"/>
+      <c r="DZ65535" s="0"/>
+      <c r="EA65535" s="0"/>
+      <c r="EB65535" s="0"/>
+      <c r="EC65535" s="0"/>
+      <c r="ED65535" s="0"/>
+      <c r="EE65535" s="0"/>
+      <c r="EF65535" s="0"/>
+      <c r="EG65535" s="0"/>
+      <c r="EH65535" s="0"/>
+      <c r="EI65535" s="0"/>
+      <c r="EJ65535" s="0"/>
+      <c r="EK65535" s="0"/>
+      <c r="EL65535" s="0"/>
+      <c r="EM65535" s="0"/>
+      <c r="EN65535" s="0"/>
+      <c r="EO65535" s="0"/>
+      <c r="EP65535" s="0"/>
+      <c r="EQ65535" s="0"/>
+      <c r="ER65535" s="0"/>
+      <c r="ES65535" s="0"/>
+      <c r="ET65535" s="0"/>
+      <c r="EU65535" s="0"/>
+      <c r="EV65535" s="0"/>
+      <c r="EW65535" s="0"/>
+      <c r="EX65535" s="0"/>
+      <c r="EY65535" s="0"/>
+      <c r="EZ65535" s="0"/>
+      <c r="FA65535" s="0"/>
+      <c r="FB65535" s="0"/>
+      <c r="FC65535" s="0"/>
+      <c r="FD65535" s="0"/>
+      <c r="FE65535" s="0"/>
+      <c r="FF65535" s="0"/>
+      <c r="FG65535" s="0"/>
+      <c r="FH65535" s="0"/>
+      <c r="FI65535" s="0"/>
+      <c r="FJ65535" s="0"/>
+      <c r="FK65535" s="0"/>
+      <c r="FL65535" s="0"/>
+      <c r="FM65535" s="0"/>
+      <c r="FN65535" s="0"/>
+      <c r="FO65535" s="0"/>
+      <c r="FP65535" s="0"/>
+      <c r="FQ65535" s="0"/>
+      <c r="FR65535" s="0"/>
+      <c r="FS65535" s="0"/>
+      <c r="FT65535" s="0"/>
+      <c r="FU65535" s="0"/>
+      <c r="FV65535" s="0"/>
+      <c r="FW65535" s="0"/>
+      <c r="FX65535" s="0"/>
+      <c r="FY65535" s="0"/>
+      <c r="FZ65535" s="0"/>
+      <c r="GA65535" s="0"/>
+      <c r="GB65535" s="0"/>
+      <c r="GC65535" s="0"/>
+      <c r="GD65535" s="0"/>
+      <c r="GE65535" s="0"/>
+      <c r="GF65535" s="0"/>
+      <c r="GG65535" s="0"/>
+      <c r="GH65535" s="0"/>
+      <c r="GI65535" s="0"/>
+      <c r="GJ65535" s="0"/>
+      <c r="GK65535" s="0"/>
+      <c r="GL65535" s="0"/>
+      <c r="GM65535" s="0"/>
+      <c r="GN65535" s="0"/>
+      <c r="GO65535" s="0"/>
+      <c r="GP65535" s="0"/>
+      <c r="GQ65535" s="0"/>
+      <c r="GR65535" s="0"/>
+      <c r="GS65535" s="0"/>
+      <c r="GT65535" s="0"/>
+      <c r="GU65535" s="0"/>
+      <c r="GV65535" s="0"/>
+      <c r="GW65535" s="0"/>
+      <c r="GX65535" s="0"/>
+      <c r="GY65535" s="0"/>
+      <c r="GZ65535" s="0"/>
+      <c r="HA65535" s="0"/>
+      <c r="HB65535" s="0"/>
+      <c r="HC65535" s="0"/>
+      <c r="HD65535" s="0"/>
+      <c r="HE65535" s="0"/>
+      <c r="HF65535" s="0"/>
+      <c r="HG65535" s="0"/>
+      <c r="HH65535" s="0"/>
+      <c r="HI65535" s="0"/>
+      <c r="HJ65535" s="0"/>
+      <c r="HK65535" s="0"/>
+      <c r="HL65535" s="0"/>
+      <c r="HM65535" s="0"/>
+      <c r="HN65535" s="0"/>
+      <c r="HO65535" s="0"/>
+      <c r="HP65535" s="0"/>
+      <c r="HQ65535" s="0"/>
+      <c r="HR65535" s="0"/>
+      <c r="HS65535" s="0"/>
+      <c r="HT65535" s="0"/>
+      <c r="HU65535" s="0"/>
+      <c r="HV65535" s="0"/>
+      <c r="HW65535" s="0"/>
+      <c r="HX65535" s="0"/>
+      <c r="HY65535" s="0"/>
+      <c r="HZ65535" s="0"/>
+      <c r="IA65535" s="0"/>
+      <c r="IB65535" s="0"/>
+      <c r="IC65535" s="0"/>
+      <c r="ID65535" s="0"/>
+      <c r="IE65535" s="0"/>
+      <c r="IF65535" s="0"/>
+      <c r="IG65535" s="0"/>
+      <c r="IH65535" s="0"/>
+      <c r="II65535" s="0"/>
+      <c r="IJ65535" s="0"/>
+      <c r="IK65535" s="0"/>
+      <c r="IL65535" s="0"/>
+      <c r="IM65535" s="0"/>
+      <c r="IN65535" s="0"/>
+      <c r="IO65535" s="0"/>
+      <c r="IP65535" s="0"/>
+      <c r="IQ65535" s="0"/>
+      <c r="IR65535" s="0"/>
+      <c r="IS65535" s="0"/>
+      <c r="IT65535" s="0"/>
+      <c r="IU65535" s="0"/>
+      <c r="IV65535" s="0"/>
+    </row>
+    <row r="65536" spans="1:256">
+      <c r="A65536" s="0"/>
+      <c r="B65536" s="0"/>
+      <c r="C65536" s="0"/>
+      <c r="D65536" s="0"/>
+      <c r="E65536" s="0"/>
+      <c r="F65536" s="0"/>
+      <c r="G65536" s="0"/>
+      <c r="H65536" s="0"/>
+      <c r="I65536" s="0"/>
+      <c r="J65536" s="0"/>
+      <c r="K65536" s="0"/>
+      <c r="L65536" s="0"/>
+      <c r="M65536" s="0"/>
+      <c r="N65536" s="0"/>
+      <c r="O65536" s="0"/>
+      <c r="P65536" s="0"/>
+      <c r="Q65536" s="0"/>
+      <c r="R65536" s="0"/>
+      <c r="S65536" s="0"/>
+      <c r="T65536" s="0"/>
+      <c r="U65536" s="0"/>
+      <c r="V65536" s="0"/>
+      <c r="W65536" s="0"/>
+      <c r="X65536" s="0"/>
+      <c r="Y65536" s="0"/>
+      <c r="Z65536" s="0"/>
+      <c r="AA65536" s="0"/>
+      <c r="AB65536" s="0"/>
+      <c r="AC65536" s="0"/>
+      <c r="AD65536" s="0"/>
+      <c r="AE65536" s="0"/>
+      <c r="AF65536" s="0"/>
+      <c r="AG65536" s="0"/>
+      <c r="AH65536" s="0"/>
+      <c r="AI65536" s="0"/>
+      <c r="AJ65536" s="0"/>
+      <c r="AK65536" s="0"/>
+      <c r="AL65536" s="0"/>
+      <c r="AM65536" s="0"/>
+      <c r="AN65536" s="0"/>
+      <c r="AO65536" s="0"/>
+      <c r="AP65536" s="0"/>
+      <c r="AQ65536" s="0"/>
+      <c r="AR65536" s="0"/>
+      <c r="AS65536" s="0"/>
+      <c r="AT65536" s="0"/>
+      <c r="AU65536" s="0"/>
+      <c r="AV65536" s="0"/>
+      <c r="AW65536" s="0"/>
+      <c r="AX65536" s="0"/>
+      <c r="AY65536" s="0"/>
+      <c r="AZ65536" s="0"/>
+      <c r="BA65536" s="0"/>
+      <c r="BB65536" s="0"/>
+      <c r="BC65536" s="0"/>
+      <c r="BD65536" s="0"/>
+      <c r="BE65536" s="0"/>
+      <c r="BF65536" s="0"/>
+      <c r="BG65536" s="0"/>
+      <c r="BH65536" s="0"/>
+      <c r="BI65536" s="0"/>
+      <c r="BJ65536" s="0"/>
+      <c r="BK65536" s="0"/>
+      <c r="BL65536" s="0"/>
+      <c r="BM65536" s="0"/>
+      <c r="BN65536" s="0"/>
+      <c r="BO65536" s="0"/>
+      <c r="BP65536" s="0"/>
+      <c r="BQ65536" s="0"/>
+      <c r="BR65536" s="0"/>
+      <c r="BS65536" s="0"/>
+      <c r="BT65536" s="0"/>
+      <c r="BU65536" s="0"/>
+      <c r="BV65536" s="0"/>
+      <c r="BW65536" s="0"/>
+      <c r="BX65536" s="0"/>
+      <c r="BY65536" s="0"/>
+      <c r="BZ65536" s="0"/>
+      <c r="CA65536" s="0"/>
+      <c r="CB65536" s="0"/>
+      <c r="CC65536" s="0"/>
+      <c r="CD65536" s="0"/>
+      <c r="CE65536" s="0"/>
+      <c r="CF65536" s="0"/>
+      <c r="CG65536" s="0"/>
+      <c r="CH65536" s="0"/>
+      <c r="CI65536" s="0"/>
+      <c r="CJ65536" s="0"/>
+      <c r="CK65536" s="0"/>
+      <c r="CL65536" s="0"/>
+      <c r="CM65536" s="0"/>
+      <c r="CN65536" s="0"/>
+      <c r="CO65536" s="0"/>
+      <c r="CP65536" s="0"/>
+      <c r="CQ65536" s="0"/>
+      <c r="CR65536" s="0"/>
+      <c r="CS65536" s="0"/>
+      <c r="CT65536" s="0"/>
+      <c r="CU65536" s="0"/>
+      <c r="CV65536" s="0"/>
+      <c r="CW65536" s="0"/>
+      <c r="CX65536" s="0"/>
+      <c r="CY65536" s="0"/>
+      <c r="CZ65536" s="0"/>
+      <c r="DA65536" s="0"/>
+      <c r="DB65536" s="0"/>
+      <c r="DC65536" s="0"/>
+      <c r="DD65536" s="0"/>
+      <c r="DE65536" s="0"/>
+      <c r="DF65536" s="0"/>
+      <c r="DG65536" s="0"/>
+      <c r="DH65536" s="0"/>
+      <c r="DI65536" s="0"/>
+      <c r="DJ65536" s="0"/>
+      <c r="DK65536" s="0"/>
+      <c r="DL65536" s="0"/>
+      <c r="DM65536" s="0"/>
+      <c r="DN65536" s="0"/>
+      <c r="DO65536" s="0"/>
+      <c r="DP65536" s="0"/>
+      <c r="DQ65536" s="0"/>
+      <c r="DR65536" s="0"/>
+      <c r="DS65536" s="0"/>
+      <c r="DT65536" s="0"/>
+      <c r="DU65536" s="0"/>
+      <c r="DV65536" s="0"/>
+      <c r="DW65536" s="0"/>
+      <c r="DX65536" s="0"/>
+      <c r="DY65536" s="0"/>
+      <c r="DZ65536" s="0"/>
+      <c r="EA65536" s="0"/>
+      <c r="EB65536" s="0"/>
+      <c r="EC65536" s="0"/>
+      <c r="ED65536" s="0"/>
+      <c r="EE65536" s="0"/>
+      <c r="EF65536" s="0"/>
+      <c r="EG65536" s="0"/>
+      <c r="EH65536" s="0"/>
+      <c r="EI65536" s="0"/>
+      <c r="EJ65536" s="0"/>
+      <c r="EK65536" s="0"/>
+      <c r="EL65536" s="0"/>
+      <c r="EM65536" s="0"/>
+      <c r="EN65536" s="0"/>
+      <c r="EO65536" s="0"/>
+      <c r="EP65536" s="0"/>
+      <c r="EQ65536" s="0"/>
+      <c r="ER65536" s="0"/>
+      <c r="ES65536" s="0"/>
+      <c r="ET65536" s="0"/>
+      <c r="EU65536" s="0"/>
+      <c r="EV65536" s="0"/>
+      <c r="EW65536" s="0"/>
+      <c r="EX65536" s="0"/>
+      <c r="EY65536" s="0"/>
+      <c r="EZ65536" s="0"/>
+      <c r="FA65536" s="0"/>
+      <c r="FB65536" s="0"/>
+      <c r="FC65536" s="0"/>
+      <c r="FD65536" s="0"/>
+      <c r="FE65536" s="0"/>
+      <c r="FF65536" s="0"/>
+      <c r="FG65536" s="0"/>
+      <c r="FH65536" s="0"/>
+      <c r="FI65536" s="0"/>
+      <c r="FJ65536" s="0"/>
+      <c r="FK65536" s="0"/>
+      <c r="FL65536" s="0"/>
+      <c r="FM65536" s="0"/>
+      <c r="FN65536" s="0"/>
+      <c r="FO65536" s="0"/>
+      <c r="FP65536" s="0"/>
+      <c r="FQ65536" s="0"/>
+      <c r="FR65536" s="0"/>
+      <c r="FS65536" s="0"/>
+      <c r="FT65536" s="0"/>
+      <c r="FU65536" s="0"/>
+      <c r="FV65536" s="0"/>
+      <c r="FW65536" s="0"/>
+      <c r="FX65536" s="0"/>
+      <c r="FY65536" s="0"/>
+      <c r="FZ65536" s="0"/>
+      <c r="GA65536" s="0"/>
+      <c r="GB65536" s="0"/>
+      <c r="GC65536" s="0"/>
+      <c r="GD65536" s="0"/>
+      <c r="GE65536" s="0"/>
+      <c r="GF65536" s="0"/>
+      <c r="GG65536" s="0"/>
+      <c r="GH65536" s="0"/>
+      <c r="GI65536" s="0"/>
+      <c r="GJ65536" s="0"/>
+      <c r="GK65536" s="0"/>
+      <c r="GL65536" s="0"/>
+      <c r="GM65536" s="0"/>
+      <c r="GN65536" s="0"/>
+      <c r="GO65536" s="0"/>
+      <c r="GP65536" s="0"/>
+      <c r="GQ65536" s="0"/>
+      <c r="GR65536" s="0"/>
+      <c r="GS65536" s="0"/>
+      <c r="GT65536" s="0"/>
+      <c r="GU65536" s="0"/>
+      <c r="GV65536" s="0"/>
+      <c r="GW65536" s="0"/>
+      <c r="GX65536" s="0"/>
+      <c r="GY65536" s="0"/>
+      <c r="GZ65536" s="0"/>
+      <c r="HA65536" s="0"/>
+      <c r="HB65536" s="0"/>
+      <c r="HC65536" s="0"/>
+      <c r="HD65536" s="0"/>
+      <c r="HE65536" s="0"/>
+      <c r="HF65536" s="0"/>
+      <c r="HG65536" s="0"/>
+      <c r="HH65536" s="0"/>
+      <c r="HI65536" s="0"/>
+      <c r="HJ65536" s="0"/>
+      <c r="HK65536" s="0"/>
+      <c r="HL65536" s="0"/>
+      <c r="HM65536" s="0"/>
+      <c r="HN65536" s="0"/>
+      <c r="HO65536" s="0"/>
+      <c r="HP65536" s="0"/>
+      <c r="HQ65536" s="0"/>
+      <c r="HR65536" s="0"/>
+      <c r="HS65536" s="0"/>
+      <c r="HT65536" s="0"/>
+      <c r="HU65536" s="0"/>
+      <c r="HV65536" s="0"/>
+      <c r="HW65536" s="0"/>
+      <c r="HX65536" s="0"/>
+      <c r="HY65536" s="0"/>
+      <c r="HZ65536" s="0"/>
+      <c r="IA65536" s="0"/>
+      <c r="IB65536" s="0"/>
+      <c r="IC65536" s="0"/>
+      <c r="ID65536" s="0"/>
+      <c r="IE65536" s="0"/>
+      <c r="IF65536" s="0"/>
+      <c r="IG65536" s="0"/>
+      <c r="IH65536" s="0"/>
+      <c r="II65536" s="0"/>
+      <c r="IJ65536" s="0"/>
+      <c r="IK65536" s="0"/>
+      <c r="IL65536" s="0"/>
+      <c r="IM65536" s="0"/>
+      <c r="IN65536" s="0"/>
+      <c r="IO65536" s="0"/>
+      <c r="IP65536" s="0"/>
+      <c r="IQ65536" s="0"/>
+      <c r="IR65536" s="0"/>
+      <c r="IS65536" s="0"/>
+      <c r="IT65536" s="0"/>
+      <c r="IU65536" s="0"/>
+      <c r="IV65536" s="0"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>